<commit_message>
970724 - +2232 - vbmellat part sell
</commit_message>
<xml_diff>
--- a/Sellbuy.xlsx
+++ b/Sellbuy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9420027-4548-4D30-9F29-1A4DB4CA4D65}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34A6274-D2A8-47B1-91CE-EE9EFB49FAA8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="F3" s="69">
         <f>SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&gt;0",Sheet3!K3:K18,"&gt;0")</f>
-        <v>629718.97320994735</v>
+        <v>4809371.036029011</v>
       </c>
       <c r="G3" s="70"/>
       <c r="I3" s="56"/>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="F4" s="67">
         <f>ABS(SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&lt;0",Sheet3!K3:K18,"&gt;0"))</f>
-        <v>4249374.9365835488</v>
+        <v>8618281.5607718229</v>
       </c>
       <c r="G4" s="68"/>
       <c r="I4" s="64" t="s">
@@ -1850,7 +1850,7 @@
       <c r="J4" s="65"/>
       <c r="K4" s="65">
         <f>DATEDIF(Sheet2!B4,F7,"d")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="66"/>
     </row>
@@ -1869,17 +1869,17 @@
       </c>
       <c r="F5" s="71">
         <f>F3-F4</f>
-        <v>-3619655.9633736014</v>
+        <v>-3808910.5247428119</v>
       </c>
       <c r="G5" s="72"/>
       <c r="I5" s="58">
         <f>((C14*100)/C13)-100</f>
-        <v>-0.87793587628731018</v>
+        <v>-1.0465554954956815</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="58">
         <f>((C14*100)/C12)-100</f>
-        <v>-0.85470781324170275</v>
+        <v>-0.69707992712609723</v>
       </c>
       <c r="L5" s="59"/>
     </row>
@@ -1912,7 +1912,7 @@
         <v>290</v>
       </c>
       <c r="F7" s="73">
-        <v>35634</v>
+        <v>35635</v>
       </c>
       <c r="G7" s="73"/>
       <c r="I7" s="62"/>
@@ -1988,18 +1988,17 @@
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="4">
-        <f>2400000</f>
-        <v>2400000</v>
+        <v>17400000</v>
       </c>
       <c r="E11" s="37">
-        <v>8000</v>
+        <v>630</v>
       </c>
       <c r="F11" s="37">
-        <v>10000</v>
+        <v>850</v>
       </c>
       <c r="G11" s="37">
         <f>((F11*100)/E11)-100</f>
-        <v>25</v>
+        <v>34.92063492063491</v>
       </c>
       <c r="I11" s="37">
         <v>2300</v>
@@ -2022,7 +2021,7 @@
       <c r="B12" s="52"/>
       <c r="C12" s="4">
         <f>SUM(C10,(C8-C9))-C11</f>
-        <v>249940553.43870014</v>
+        <v>234940553.43870014</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
@@ -2032,7 +2031,7 @@
       <c r="B13" s="50"/>
       <c r="C13" s="26">
         <f>Sheet2!G19</f>
-        <v>249999124</v>
+        <v>235770297</v>
       </c>
       <c r="E13" s="51" t="s">
         <v>287</v>
@@ -2047,7 +2046,7 @@
       <c r="B14" s="50"/>
       <c r="C14" s="26">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet3!E3:E18)</f>
-        <v>247804292</v>
+        <v>233302830</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>9</v>
@@ -2066,7 +2065,7 @@
       <c r="B15" s="50"/>
       <c r="C15" s="26">
         <f>C12-C13</f>
-        <v>-58570.561299860477</v>
+        <v>-829743.56129986048</v>
       </c>
       <c r="E15" s="38" t="s">
         <v>293</v>
@@ -2116,7 +2115,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2563,7 @@
       </c>
       <c r="H14" s="11">
         <f>IF(Sheet3!K14,(G14*100)/G19,0)</f>
-        <v>39.997983352933666</v>
+        <v>42.41187684469007</v>
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
@@ -2579,25 +2578,25 @@
         <v>35628</v>
       </c>
       <c r="C15" s="6">
-        <v>43276</v>
+        <v>37119</v>
       </c>
       <c r="D15" s="40">
         <v>2300</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>99534800</v>
+        <v>85373700</v>
       </c>
       <c r="F15" s="40">
         <v>2311</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="2"/>
-        <v>100010836</v>
+        <v>85782009</v>
       </c>
       <c r="H15" s="11">
         <f>IF(Sheet3!K15,(G15*100)/G19,0)</f>
-        <v>40.004474575678913</v>
+        <v>36.383721822261606</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
@@ -2630,7 +2629,7 @@
       </c>
       <c r="H16" s="11">
         <f>IF(Sheet3!K16,(G16*100)/G19,0)</f>
-        <v>19.997542071387418</v>
+        <v>21.204401333048327</v>
       </c>
       <c r="I16" s="41">
         <f t="shared" si="1"/>
@@ -2688,7 +2687,7 @@
       <c r="F19" s="76"/>
       <c r="G19" s="17">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet2!G3:G18)</f>
-        <v>249999124</v>
+        <v>235770297</v>
       </c>
       <c r="H19" s="17">
         <f>SUM(H4:H18)</f>
@@ -2709,7 +2708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8F56D5-BF3E-49D5-B38A-3E5EE968ED27}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3246,38 +3245,38 @@
         <v>15</v>
       </c>
       <c r="B14" s="42">
-        <v>35634</v>
+        <v>35635</v>
       </c>
       <c r="C14" s="6">
         <f>Sheet2!C14</f>
         <v>9288</v>
       </c>
       <c r="D14" s="40">
-        <v>10376</v>
+        <v>9895</v>
       </c>
       <c r="E14" s="40">
         <f t="shared" si="0"/>
-        <v>96372288</v>
+        <v>91904760</v>
       </c>
       <c r="F14" s="40">
         <f t="shared" si="1"/>
-        <v>554120.9324475379</v>
+        <v>528433.56077181839</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" ref="G14:G16" si="3">E14-F14</f>
-        <v>95818167.067552462</v>
+        <v>91376326.439228177</v>
       </c>
       <c r="H14" s="19">
         <f>DATEDIF(Sheet2!B14,B14,"d")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I14" s="24">
         <f>((G14*100)/Sheet2!G14)-100</f>
-        <v>-4.1766661382857109</v>
+        <v>-8.6187462835714399</v>
       </c>
       <c r="J14" s="20">
         <f>Sheet3!G14-Sheet2!G14</f>
-        <v>-4176440.9324475378</v>
+        <v>-8618281.5607718229</v>
       </c>
       <c r="K14" s="27">
         <v>1</v>
@@ -3288,38 +3287,38 @@
         <v>50</v>
       </c>
       <c r="B15" s="48">
-        <v>35634</v>
+        <v>35635</v>
       </c>
       <c r="C15" s="6">
         <f>Sheet2!C15</f>
-        <v>43276</v>
+        <v>37119</v>
       </c>
       <c r="D15" s="40">
-        <v>2339</v>
+        <v>2450</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>101222564</v>
+        <v>90941550</v>
       </c>
       <c r="F15" s="40">
         <f t="shared" si="1"/>
-        <v>582009.02679005172</v>
+        <v>522895.30040237698</v>
       </c>
       <c r="G15" s="40">
         <f t="shared" si="3"/>
-        <v>100640554.97320995</v>
+        <v>90418654.699597627</v>
       </c>
       <c r="H15" s="19">
         <f>DATEDIF(Sheet2!B15,B15,"d")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I15" s="24">
         <f>((G15*100)/Sheet2!G15)-100</f>
-        <v>0.62965074425530076</v>
+        <v>5.4051493473388206</v>
       </c>
       <c r="J15" s="20">
         <f>Sheet3!G15-Sheet2!G15</f>
-        <v>629718.97320994735</v>
+        <v>4636645.6995976269</v>
       </c>
       <c r="K15" s="27">
         <v>1</v>
@@ -3330,37 +3329,37 @@
         <v>292</v>
       </c>
       <c r="B16" s="48">
-        <v>35634</v>
+        <v>35635</v>
       </c>
       <c r="C16" s="6">
         <v>3480</v>
       </c>
       <c r="D16" s="41">
-        <v>14428</v>
+        <v>14499</v>
       </c>
       <c r="E16" s="41">
         <f t="shared" si="0"/>
-        <v>50209440</v>
+        <v>50456520</v>
       </c>
       <c r="F16" s="41">
         <f t="shared" si="1"/>
-        <v>288694.00413600961</v>
+        <v>290114.66356861679</v>
       </c>
       <c r="G16" s="41">
         <f t="shared" si="3"/>
-        <v>49920745.995863989</v>
+        <v>50166405.336431384</v>
       </c>
       <c r="H16" s="19">
         <f>DATEDIF(Sheet2!B16,B16,"d")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="24">
         <f>((G16*100)/Sheet2!G16)-100</f>
-        <v>-0.14588644831908937</v>
+        <v>0.34549434334778084</v>
       </c>
       <c r="J16" s="20">
         <f>Sheet3!G16-Sheet2!G16</f>
-        <v>-72934.004136011004</v>
+        <v>172725.33643138409</v>
       </c>
       <c r="K16" s="17">
         <v>1</v>
@@ -3403,7 +3402,7 @@
       <c r="F19" s="81"/>
       <c r="G19" s="84">
         <f>SUMIF(K3:K18,"&gt;0",G3:G18)</f>
-        <v>246379468.0366264</v>
+        <v>231961386.47525719</v>
       </c>
       <c r="H19" s="84"/>
       <c r="I19" s="84"/>

</xml_diff>

<commit_message>
970805 - -2200 vbmellat part sell
روز بد بورس تکرار شد و شاخص افت شدید پیدا کرد
هر سه سهم سبد با صف فروش همراه شدند
</commit_message>
<xml_diff>
--- a/Sellbuy.xlsx
+++ b/Sellbuy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D46F7C-3F2D-41CD-9B07-27CFCAF4D04E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FBADF3-B346-408D-9584-F4EE8A5D80EB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="293">
   <si>
     <t>آورده نقدی</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>وضعیت</t>
-  </si>
-  <si>
-    <t>باقیمانده حساب آگاه</t>
   </si>
   <si>
     <t>ضرر سهام</t>
@@ -1367,79 +1364,79 @@
     <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1771,7 +1768,7 @@
   <dimension ref="A2:L15"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,24 +1782,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="E2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="52"/>
-      <c r="I2" s="54" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="I2" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="54" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="55"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
@@ -1817,15 +1814,15 @@
       <c r="E3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="69">
+      <c r="F3" s="67">
         <f>SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&gt;0",Sheet3!K3:K18,"&gt;0")</f>
-        <v>7220035.8338718414</v>
-      </c>
-      <c r="G3" s="70"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="57"/>
+        <v>2154427.2533821166</v>
+      </c>
+      <c r="G3" s="68"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1840,20 +1837,20 @@
       <c r="E4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="65">
         <f>ABS(SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&lt;0",Sheet3!K3:K18,"&gt;0"))</f>
-        <v>10050180.606642038</v>
-      </c>
-      <c r="G4" s="68"/>
-      <c r="I4" s="64" t="s">
+        <v>14583245.679744273</v>
+      </c>
+      <c r="G4" s="66"/>
+      <c r="I4" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65">
+      <c r="J4" s="63"/>
+      <c r="K4" s="63">
         <f>DATEDIF(Sheet2!B4,F7,"d")-1</f>
-        <v>36</v>
-      </c>
-      <c r="L4" s="66"/>
+        <v>39</v>
+      </c>
+      <c r="L4" s="64"/>
     </row>
     <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
@@ -1868,21 +1865,21 @@
       <c r="E5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="71">
+      <c r="F5" s="69">
         <f>F3-F4</f>
-        <v>-2830144.7727701962</v>
-      </c>
-      <c r="G5" s="72"/>
-      <c r="I5" s="58">
+        <v>-12428818.426362157</v>
+      </c>
+      <c r="G5" s="70"/>
+      <c r="I5" s="56">
         <f>((C14*100)/C13)-100</f>
-        <v>-0.62901943920442704</v>
-      </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="58">
+        <v>-4.9460428960216234</v>
+      </c>
+      <c r="J5" s="57"/>
+      <c r="K5" s="56">
         <f>((C14*100)/C12)-100</f>
-        <v>-0.27806925162053631</v>
-      </c>
-      <c r="L5" s="59"/>
+        <v>-4.3784890221603092</v>
+      </c>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
@@ -1894,10 +1891,10 @@
       <c r="C6" s="2">
         <v>30000000</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="61"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -1910,22 +1907,22 @@
         <v>70000000</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>290</v>
-      </c>
-      <c r="F7" s="73">
-        <v>35644</v>
-      </c>
-      <c r="G7" s="73"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
+        <v>289</v>
+      </c>
+      <c r="F7" s="71">
+        <v>35647</v>
+      </c>
+      <c r="G7" s="71"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="52"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="4">
         <f>SUMIFS(Sheet3!J3:J18,Sheet3!K3:K18,"=0",Sheet3!J3:J18,"&gt;0")</f>
         <v>26800150.399080981</v>
@@ -1933,30 +1930,30 @@
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="52"/>
+        <v>48</v>
+      </c>
+      <c r="B9" s="50"/>
       <c r="C9" s="4">
         <f>ABS(SUMIFS(Sheet3!J3:J18,Sheet3!K3:K18,"=0",Sheet3!J3:J18,"&lt;0"))</f>
         <v>24459596.960380837</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>280</v>
-      </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="52"/>
+        <v>279</v>
+      </c>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
       <c r="I9" s="51" t="s">
-        <v>283</v>
-      </c>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="52"/>
+        <v>282</v>
+      </c>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="4">
         <f>SUM(C4:C7)</f>
         <v>250000000</v>
@@ -1965,31 +1962,31 @@
         <v>8</v>
       </c>
       <c r="F10" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="32" t="s">
         <v>281</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>282</v>
       </c>
       <c r="I10" s="32" t="s">
         <v>8</v>
       </c>
       <c r="J10" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="K10" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="L10" s="32" t="s">
         <v>285</v>
-      </c>
-      <c r="L10" s="32" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="51" t="s">
-        <v>291</v>
-      </c>
-      <c r="B11" s="52"/>
+        <v>290</v>
+      </c>
+      <c r="B11" s="50"/>
       <c r="C11" s="4">
-        <v>17400000</v>
+        <v>27400000</v>
       </c>
       <c r="E11" s="37">
         <v>410</v>
@@ -2019,57 +2016,52 @@
       <c r="A12" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="52"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="4">
         <f>SUM(C10,(C8-C9))-C11</f>
-        <v>234940553.43870014</v>
+        <v>224940553.43870014</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="50"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="26">
         <f>Sheet2!G19</f>
-        <v>235770297</v>
+        <v>226283642</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>287</v>
-      </c>
-      <c r="F13" s="53"/>
-      <c r="G13" s="52"/>
+        <v>286</v>
+      </c>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="26">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet3!E3:E18)</f>
-        <v>234287256</v>
+        <v>215091556</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="G14" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="G14" s="32" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="15" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A15" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="26">
-        <f>C12-C13</f>
-        <v>-829743.56129986048</v>
-      </c>
+      <c r="A15" s="72"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="26"/>
       <c r="E15" s="38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F15" s="37" t="b">
         <f>ISNUMBER(SEARCH(E15,Sheet4!A:A))</f>
@@ -2082,6 +2074,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:L9"/>
@@ -2098,13 +2097,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2116,7 +2108,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,7 +2499,7 @@
     </row>
     <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="14">
         <v>35625</v>
@@ -2564,7 +2556,7 @@
       </c>
       <c r="H14" s="11">
         <f>IF(Sheet3!K14,(G14*100)/G19,0)</f>
-        <v>42.41187684469007</v>
+        <v>44.189941047528308</v>
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
@@ -2573,31 +2565,31 @@
     </row>
     <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="12">
         <v>35628</v>
       </c>
       <c r="C15" s="6">
-        <v>37119</v>
+        <v>33014</v>
       </c>
       <c r="D15" s="40">
         <v>2300</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>85373700</v>
+        <v>75932200</v>
       </c>
       <c r="F15" s="40">
         <v>2311</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="2"/>
-        <v>85782009</v>
+        <v>76295354</v>
       </c>
       <c r="H15" s="11">
         <f>IF(Sheet3!K15,(G15*100)/G19,0)</f>
-        <v>36.383721822261606</v>
+        <v>33.716689958525592</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
@@ -2606,7 +2598,7 @@
     </row>
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B16" s="42">
         <v>35629</v>
@@ -2630,7 +2622,7 @@
       </c>
       <c r="H16" s="11">
         <f>IF(Sheet3!K16,(G16*100)/G19,0)</f>
-        <v>21.204401333048327</v>
+        <v>22.093368993946104</v>
       </c>
       <c r="I16" s="41">
         <f t="shared" si="1"/>
@@ -2688,7 +2680,7 @@
       <c r="F19" s="76"/>
       <c r="G19" s="17">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet2!G3:G18)</f>
-        <v>235770297</v>
+        <v>226283642</v>
       </c>
       <c r="H19" s="17">
         <f>SUM(H4:H18)</f>
@@ -2710,7 +2702,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -3201,7 +3193,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="14">
         <v>35627</v>
@@ -3246,38 +3238,38 @@
         <v>15</v>
       </c>
       <c r="B14" s="42">
-        <v>35644</v>
+        <v>35647</v>
       </c>
       <c r="C14" s="6">
         <f>Sheet2!C14</f>
         <v>9288</v>
       </c>
       <c r="D14" s="40">
-        <v>9852</v>
+        <v>9502</v>
       </c>
       <c r="E14" s="40">
         <f t="shared" si="0"/>
-        <v>91505376</v>
+        <v>88254576</v>
       </c>
       <c r="F14" s="40">
         <f t="shared" si="1"/>
-        <v>526137.18450974778</v>
+        <v>507445.7498184758</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" ref="G14:G16" si="3">E14-F14</f>
-        <v>90979238.815490246</v>
+        <v>87747130.250181526</v>
       </c>
       <c r="H14" s="19">
         <f>DATEDIF(Sheet2!B14,B14,"d")-1</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I14" s="24">
         <f>((G14*100)/Sheet2!G14)-100</f>
-        <v>-9.0158553194285815</v>
+        <v>-12.248138169428572</v>
       </c>
       <c r="J14" s="20">
         <f>Sheet3!G14-Sheet2!G14</f>
-        <v>-9015369.1845097542</v>
+        <v>-12247477.749818474</v>
       </c>
       <c r="K14" s="27">
         <v>1</v>
@@ -3285,41 +3277,41 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="48">
-        <v>35644</v>
+        <v>35647</v>
       </c>
       <c r="C15" s="6">
         <f>Sheet2!C15</f>
-        <v>37119</v>
+        <v>33014</v>
       </c>
       <c r="D15" s="40">
-        <v>2520</v>
+        <v>2390</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>93539880</v>
+        <v>78903460</v>
       </c>
       <c r="F15" s="40">
         <f t="shared" si="1"/>
-        <v>537835.16612815915</v>
+        <v>453678.7466178764</v>
       </c>
       <c r="G15" s="40">
         <f t="shared" si="3"/>
-        <v>93002044.833871841</v>
+        <v>78449781.253382117</v>
       </c>
       <c r="H15" s="19">
         <f>DATEDIF(Sheet2!B15,B15,"d")-1</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I15" s="24">
         <f>((G15*100)/Sheet2!G15)-100</f>
-        <v>8.4167250429770633</v>
+        <v>2.8237987510774474</v>
       </c>
       <c r="J15" s="20">
         <f>Sheet3!G15-Sheet2!G15</f>
-        <v>7220035.8338718414</v>
+        <v>2154427.2533821166</v>
       </c>
       <c r="K15" s="27">
         <v>1</v>
@@ -3327,40 +3319,40 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B16" s="48">
-        <v>35644</v>
+        <v>35647</v>
       </c>
       <c r="C16" s="6">
         <v>3480</v>
       </c>
       <c r="D16" s="41">
-        <v>14150</v>
+        <v>13774</v>
       </c>
       <c r="E16" s="41">
         <f t="shared" si="0"/>
-        <v>49242000</v>
+        <v>47933520</v>
       </c>
       <c r="F16" s="41">
         <f t="shared" si="1"/>
-        <v>283131.42213228001</v>
+        <v>275607.92992579681</v>
       </c>
       <c r="G16" s="41">
         <f t="shared" si="3"/>
-        <v>48958868.577867717</v>
+        <v>47657912.070074201</v>
       </c>
       <c r="H16" s="19">
         <f>DATEDIF(Sheet2!B16,B16,"d")-1</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I16" s="24">
         <f>((G16*100)/Sheet2!G16)-100</f>
-        <v>-2.0698844776625407</v>
+        <v>-4.6721264166306753</v>
       </c>
       <c r="J16" s="20">
         <f>Sheet3!G16-Sheet2!G16</f>
-        <v>-1034811.4221322834</v>
+        <v>-2335767.9299257994</v>
       </c>
       <c r="K16" s="17">
         <v>1</v>
@@ -3403,7 +3395,7 @@
       <c r="F19" s="81"/>
       <c r="G19" s="84">
         <f>SUMIF(K3:K18,"&gt;0",G3:G18)</f>
-        <v>232940152.2272298</v>
+        <v>213854823.57363784</v>
       </c>
       <c r="H19" s="84"/>
       <c r="I19" s="84"/>
@@ -3443,10 +3435,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>252</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3454,24 +3446,24 @@
         <v>9</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="34">
         <v>1</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="34">
         <v>1</v>
@@ -3479,13 +3471,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="35">
         <v>2</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="35">
         <v>2</v>
@@ -3493,13 +3485,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="34">
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="34">
         <v>3</v>
@@ -3507,13 +3499,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="35">
         <v>4</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="35">
         <v>4</v>
@@ -3521,13 +3513,13 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="34">
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="34">
         <v>5</v>
@@ -3535,13 +3527,13 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="35">
         <v>6</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="35">
         <v>6</v>
@@ -3549,13 +3541,13 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="34">
         <v>7</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="34">
         <v>7</v>
@@ -3563,13 +3555,13 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="35">
         <v>8</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="35">
         <v>8</v>
@@ -3577,13 +3569,13 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="34">
         <v>9</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="34">
         <v>9</v>
@@ -3591,13 +3583,13 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="35">
         <v>10</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="35">
         <v>10</v>
@@ -3605,13 +3597,13 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="34">
         <v>11</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="34">
         <v>11</v>
@@ -3619,13 +3611,13 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="35">
         <v>12</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="35">
         <v>12</v>
@@ -3633,13 +3625,13 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="34">
         <v>13</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="34">
         <v>13</v>
@@ -3647,13 +3639,13 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="35">
         <v>14</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="35">
         <v>14</v>
@@ -3661,13 +3653,13 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="34">
         <v>15</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="34">
         <v>15</v>
@@ -3675,13 +3667,13 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="35">
         <v>16</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="35">
         <v>16</v>
@@ -3689,13 +3681,13 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="34">
         <v>17</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="34">
         <v>17</v>
@@ -3703,13 +3695,13 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="35">
         <v>18</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="35">
         <v>18</v>
@@ -3717,13 +3709,13 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="34">
         <v>19</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="34">
         <v>19</v>
@@ -3731,13 +3723,13 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="35">
         <v>20</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="35">
         <v>20</v>
@@ -3745,13 +3737,13 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="34">
         <v>21</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="34">
         <v>21</v>
@@ -3759,13 +3751,13 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="35">
         <v>22</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="35">
         <v>22</v>
@@ -3773,13 +3765,13 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="34">
         <v>23</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" s="34">
         <v>23</v>
@@ -3787,13 +3779,13 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="35">
         <v>24</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="35">
         <v>24</v>
@@ -3801,13 +3793,13 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="34">
         <v>25</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="34">
         <v>25</v>
@@ -3815,13 +3807,13 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="35">
         <v>26</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="35">
         <v>26</v>
@@ -3829,13 +3821,13 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="34">
         <v>27</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="34">
         <v>27</v>
@@ -3843,13 +3835,13 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="35">
         <v>28</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="35">
         <v>28</v>
@@ -3857,13 +3849,13 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="34">
         <v>29</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="34">
         <v>29</v>
@@ -3871,13 +3863,13 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="35">
         <v>30</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="35">
         <v>30</v>
@@ -3885,13 +3877,13 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="34">
         <v>31</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="34">
         <v>31</v>
@@ -3899,13 +3891,13 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="35">
         <v>32</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="35">
         <v>32</v>
@@ -3913,13 +3905,13 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="34">
         <v>33</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="34">
         <v>33</v>
@@ -3927,13 +3919,13 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="35">
         <v>34</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="35">
         <v>34</v>
@@ -3941,13 +3933,13 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" s="34">
         <v>35</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="34">
         <v>35</v>
@@ -3955,13 +3947,13 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="35">
         <v>36</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="35">
         <v>36</v>
@@ -3969,13 +3961,13 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="34">
         <v>37</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="34">
         <v>37</v>
@@ -3983,13 +3975,13 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="35">
         <v>38</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="35">
         <v>38</v>
@@ -3997,13 +3989,13 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="34">
         <v>39</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" s="34">
         <v>39</v>
@@ -4011,13 +4003,13 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="35">
         <v>40</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="35">
         <v>40</v>
@@ -4025,13 +4017,13 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="34">
         <v>41</v>
       </c>
       <c r="C43" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="34">
         <v>41</v>
@@ -4039,13 +4031,13 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" s="35">
         <v>42</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="35">
         <v>42</v>
@@ -4053,13 +4045,13 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" s="34">
         <v>43</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D45" s="34">
         <v>43</v>
@@ -4067,13 +4059,13 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="35">
         <v>44</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="35">
         <v>44</v>
@@ -4081,13 +4073,13 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47" s="34">
         <v>45</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D47" s="34">
         <v>45</v>
@@ -4095,13 +4087,13 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="35">
         <v>46</v>
       </c>
       <c r="C48" s="46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D48" s="35">
         <v>46</v>
@@ -4109,13 +4101,13 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="34">
         <v>47</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D49" s="34">
         <v>47</v>
@@ -4123,13 +4115,13 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="35">
         <v>48</v>
       </c>
       <c r="C50" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D50" s="35">
         <v>48</v>
@@ -4137,13 +4129,13 @@
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="34">
         <v>49</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D51" s="34">
         <v>49</v>
@@ -4151,13 +4143,13 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="35">
         <v>50</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" s="35">
         <v>50</v>
@@ -4165,13 +4157,13 @@
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="34">
         <v>51</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="34">
         <v>51</v>
@@ -4179,13 +4171,13 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="35">
         <v>52</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D54" s="35">
         <v>52</v>
@@ -4193,13 +4185,13 @@
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="34">
         <v>53</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D55" s="34">
         <v>53</v>
@@ -4207,13 +4199,13 @@
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" s="35">
         <v>54</v>
       </c>
       <c r="C56" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D56" s="35">
         <v>54</v>
@@ -4221,13 +4213,13 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="34">
         <v>55</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D57" s="34">
         <v>55</v>
@@ -4235,13 +4227,13 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="35">
         <v>56</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D58" s="35">
         <v>56</v>
@@ -4249,13 +4241,13 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="34">
         <v>57</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D59" s="34">
         <v>57</v>
@@ -4263,13 +4255,13 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="35">
         <v>58</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D60" s="35">
         <v>58</v>
@@ -4277,13 +4269,13 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="34">
         <v>59</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D61" s="34">
         <v>59</v>
@@ -4291,13 +4283,13 @@
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" s="35">
         <v>60</v>
       </c>
       <c r="C62" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D62" s="35">
         <v>60</v>
@@ -4305,13 +4297,13 @@
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B63" s="34">
         <v>61</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D63" s="34">
         <v>61</v>
@@ -4319,13 +4311,13 @@
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B64" s="35">
         <v>62</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D64" s="35">
         <v>62</v>
@@ -4333,13 +4325,13 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" s="34">
         <v>63</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" s="34">
         <v>63</v>
@@ -4347,13 +4339,13 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" s="35">
         <v>64</v>
       </c>
       <c r="C66" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="35">
         <v>64</v>
@@ -4361,13 +4353,13 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B67" s="34">
         <v>65</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D67" s="34">
         <v>65</v>
@@ -4375,13 +4367,13 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B68" s="35">
         <v>66</v>
       </c>
       <c r="C68" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="35">
         <v>66</v>
@@ -4389,13 +4381,13 @@
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B69" s="34">
         <v>67</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D69" s="34">
         <v>67</v>
@@ -4403,13 +4395,13 @@
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B70" s="35">
         <v>68</v>
       </c>
       <c r="C70" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D70" s="35">
         <v>68</v>
@@ -4417,13 +4409,13 @@
     </row>
     <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B71" s="34">
         <v>69</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D71" s="34">
         <v>69</v>
@@ -4431,13 +4423,13 @@
     </row>
     <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B72" s="35">
         <v>70</v>
       </c>
       <c r="C72" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D72" s="35">
         <v>70</v>
@@ -4445,13 +4437,13 @@
     </row>
     <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B73" s="34">
         <v>71</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D73" s="34">
         <v>71</v>
@@ -4459,13 +4451,13 @@
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B74" s="35">
         <v>72</v>
       </c>
       <c r="C74" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D74" s="35">
         <v>72</v>
@@ -4473,13 +4465,13 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B75" s="34">
         <v>73</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D75" s="34">
         <v>73</v>
@@ -4487,13 +4479,13 @@
     </row>
     <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B76" s="35">
         <v>74</v>
       </c>
       <c r="C76" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D76" s="35">
         <v>74</v>
@@ -4501,13 +4493,13 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B77" s="34">
         <v>75</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D77" s="34">
         <v>75</v>
@@ -4515,13 +4507,13 @@
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B78" s="35">
         <v>76</v>
       </c>
       <c r="C78" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D78" s="35">
         <v>76</v>
@@ -4529,13 +4521,13 @@
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" s="34">
         <v>77</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D79" s="34">
         <v>77</v>
@@ -4543,13 +4535,13 @@
     </row>
     <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B80" s="35">
         <v>78</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D80" s="35">
         <v>78</v>
@@ -4557,13 +4549,13 @@
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B81" s="34">
         <v>79</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D81" s="34">
         <v>79</v>
@@ -4571,13 +4563,13 @@
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B82" s="35">
         <v>80</v>
       </c>
       <c r="C82" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D82" s="35">
         <v>80</v>
@@ -4585,13 +4577,13 @@
     </row>
     <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B83" s="34">
         <v>81</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D83" s="34">
         <v>81</v>
@@ -4599,13 +4591,13 @@
     </row>
     <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B84" s="35">
         <v>82</v>
       </c>
       <c r="C84" s="46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D84" s="35">
         <v>82</v>
@@ -4613,13 +4605,13 @@
     </row>
     <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B85" s="34">
         <v>83</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D85" s="34">
         <v>83</v>
@@ -4627,13 +4619,13 @@
     </row>
     <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B86" s="35">
         <v>84</v>
       </c>
       <c r="C86" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D86" s="35">
         <v>84</v>
@@ -4641,13 +4633,13 @@
     </row>
     <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B87" s="34">
         <v>85</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D87" s="34">
         <v>85</v>
@@ -4655,13 +4647,13 @@
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B88" s="35">
         <v>86</v>
       </c>
       <c r="C88" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D88" s="35">
         <v>86</v>
@@ -4669,13 +4661,13 @@
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" s="34">
         <v>87</v>
       </c>
       <c r="C89" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D89" s="34">
         <v>87</v>
@@ -4683,13 +4675,13 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B90" s="35">
         <v>88</v>
       </c>
       <c r="C90" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D90" s="35">
         <v>88</v>
@@ -4697,13 +4689,13 @@
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B91" s="34">
         <v>89</v>
       </c>
       <c r="C91" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D91" s="34">
         <v>89</v>
@@ -4711,13 +4703,13 @@
     </row>
     <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B92" s="35">
         <v>90</v>
       </c>
       <c r="C92" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D92" s="35">
         <v>90</v>
@@ -4725,13 +4717,13 @@
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B93" s="34">
         <v>91</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D93" s="34">
         <v>91</v>
@@ -4739,13 +4731,13 @@
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B94" s="35">
         <v>92</v>
       </c>
       <c r="C94" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D94" s="35">
         <v>92</v>
@@ -4753,13 +4745,13 @@
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B95" s="34">
         <v>93</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D95" s="34">
         <v>93</v>
@@ -4767,13 +4759,13 @@
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B96" s="35">
         <v>94</v>
       </c>
       <c r="C96" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D96" s="35">
         <v>94</v>
@@ -4781,13 +4773,13 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B97" s="34">
         <v>95</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D97" s="34">
         <v>95</v>
@@ -4795,13 +4787,13 @@
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B98" s="35">
         <v>96</v>
       </c>
       <c r="C98" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D98" s="35">
         <v>96</v>
@@ -4809,13 +4801,13 @@
     </row>
     <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B99" s="34">
         <v>97</v>
       </c>
       <c r="C99" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D99" s="34">
         <v>97</v>
@@ -4823,13 +4815,13 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B100" s="35">
         <v>98</v>
       </c>
       <c r="C100" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D100" s="35">
         <v>98</v>
@@ -4837,13 +4829,13 @@
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B101" s="34">
         <v>99</v>
       </c>
       <c r="C101" s="45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D101" s="34">
         <v>99</v>
@@ -4851,13 +4843,13 @@
     </row>
     <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B102" s="35">
         <v>100</v>
       </c>
       <c r="C102" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D102" s="35">
         <v>100</v>
@@ -4865,13 +4857,13 @@
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B103" s="34">
         <v>101</v>
       </c>
       <c r="C103" s="45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D103" s="34">
         <v>101</v>
@@ -4879,13 +4871,13 @@
     </row>
     <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B104" s="35">
         <v>102</v>
       </c>
       <c r="C104" s="46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D104" s="35">
         <v>102</v>
@@ -4893,13 +4885,13 @@
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B105" s="34">
         <v>103</v>
       </c>
       <c r="C105" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D105" s="34">
         <v>103</v>
@@ -4907,13 +4899,13 @@
     </row>
     <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B106" s="35">
         <v>104</v>
       </c>
       <c r="C106" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D106" s="35">
         <v>104</v>
@@ -4921,13 +4913,13 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B107" s="34">
         <v>105</v>
       </c>
       <c r="C107" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D107" s="34">
         <v>105</v>
@@ -4935,13 +4927,13 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B108" s="35">
         <v>106</v>
       </c>
       <c r="C108" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D108" s="35">
         <v>106</v>
@@ -4949,13 +4941,13 @@
     </row>
     <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B109" s="34">
         <v>107</v>
       </c>
       <c r="C109" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D109" s="34">
         <v>107</v>
@@ -4963,13 +4955,13 @@
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B110" s="35">
         <v>108</v>
       </c>
       <c r="C110" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D110" s="35">
         <v>108</v>
@@ -4977,13 +4969,13 @@
     </row>
     <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B111" s="34">
         <v>109</v>
       </c>
       <c r="C111" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D111" s="34">
         <v>109</v>
@@ -4991,13 +4983,13 @@
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B112" s="35">
         <v>110</v>
       </c>
       <c r="C112" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D112" s="35">
         <v>110</v>
@@ -5005,13 +4997,13 @@
     </row>
     <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B113" s="34">
         <v>111</v>
       </c>
       <c r="C113" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D113" s="34">
         <v>111</v>
@@ -5019,13 +5011,13 @@
     </row>
     <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B114" s="35">
         <v>112</v>
       </c>
       <c r="C114" s="46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D114" s="35">
         <v>112</v>
@@ -5033,13 +5025,13 @@
     </row>
     <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B115" s="34">
         <v>113</v>
       </c>
       <c r="C115" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D115" s="34">
         <v>113</v>
@@ -5047,13 +5039,13 @@
     </row>
     <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B116" s="35">
         <v>114</v>
       </c>
       <c r="C116" s="46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D116" s="35">
         <v>114</v>
@@ -5061,13 +5053,13 @@
     </row>
     <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B117" s="34">
         <v>115</v>
       </c>
       <c r="C117" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D117" s="34">
         <v>115</v>
@@ -5075,13 +5067,13 @@
     </row>
     <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B118" s="35">
         <v>116</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D118" s="35">
         <v>116</v>
@@ -5089,13 +5081,13 @@
     </row>
     <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B119" s="34">
         <v>117</v>
       </c>
       <c r="C119" s="45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D119" s="34">
         <v>117</v>
@@ -5103,13 +5095,13 @@
     </row>
     <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B120" s="35">
         <v>118</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D120" s="35">
         <v>118</v>
@@ -5117,13 +5109,13 @@
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B121" s="34">
         <v>119</v>
       </c>
       <c r="C121" s="45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D121" s="34">
         <v>119</v>
@@ -5131,13 +5123,13 @@
     </row>
     <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B122" s="35">
         <v>120</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D122" s="35">
         <v>120</v>
@@ -5145,13 +5137,13 @@
     </row>
     <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B123" s="34">
         <v>121</v>
       </c>
       <c r="C123" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D123" s="34">
         <v>121</v>
@@ -5159,13 +5151,13 @@
     </row>
     <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B124" s="35">
         <v>122</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D124" s="35">
         <v>122</v>
@@ -5173,13 +5165,13 @@
     </row>
     <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B125" s="34">
         <v>123</v>
       </c>
       <c r="C125" s="45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D125" s="34">
         <v>123</v>
@@ -5187,13 +5179,13 @@
     </row>
     <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B126" s="35">
         <v>124</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D126" s="35">
         <v>124</v>
@@ -5201,13 +5193,13 @@
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B127" s="34">
         <v>125</v>
       </c>
       <c r="C127" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D127" s="34">
         <v>125</v>
@@ -5215,13 +5207,13 @@
     </row>
     <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B128" s="35">
         <v>126</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D128" s="35">
         <v>126</v>
@@ -5229,13 +5221,13 @@
     </row>
     <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B129" s="34">
         <v>127</v>
       </c>
       <c r="C129" s="45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D129" s="34">
         <v>127</v>
@@ -5243,13 +5235,13 @@
     </row>
     <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B130" s="35">
         <v>128</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D130" s="35">
         <v>128</v>
@@ -5257,13 +5249,13 @@
     </row>
     <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B131" s="34">
         <v>129</v>
       </c>
       <c r="C131" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D131" s="34">
         <v>129</v>
@@ -5271,13 +5263,13 @@
     </row>
     <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B132" s="35">
         <v>130</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D132" s="35">
         <v>130</v>
@@ -5285,13 +5277,13 @@
     </row>
     <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B133" s="34">
         <v>131</v>
       </c>
       <c r="C133" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D133" s="34">
         <v>131</v>
@@ -5299,13 +5291,13 @@
     </row>
     <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B134" s="35">
         <v>132</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D134" s="35">
         <v>132</v>
@@ -5313,13 +5305,13 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B135" s="34">
         <v>133</v>
       </c>
       <c r="C135" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D135" s="34">
         <v>133</v>
@@ -5327,13 +5319,13 @@
     </row>
     <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B136" s="35">
         <v>134</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D136" s="35">
         <v>134</v>
@@ -5341,13 +5333,13 @@
     </row>
     <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B137" s="34">
         <v>135</v>
       </c>
       <c r="C137" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D137" s="34">
         <v>135</v>
@@ -5355,13 +5347,13 @@
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B138" s="35">
         <v>136</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D138" s="35">
         <v>136</v>
@@ -5369,13 +5361,13 @@
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B139" s="34">
         <v>137</v>
       </c>
       <c r="C139" s="45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D139" s="34">
         <v>137</v>
@@ -5383,13 +5375,13 @@
     </row>
     <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B140" s="35">
         <v>138</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D140" s="35">
         <v>138</v>
@@ -5397,13 +5389,13 @@
     </row>
     <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B141" s="34">
         <v>139</v>
       </c>
       <c r="C141" s="45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D141" s="34">
         <v>139</v>
@@ -5411,13 +5403,13 @@
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B142" s="35">
         <v>140</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D142" s="35">
         <v>140</v>
@@ -5425,13 +5417,13 @@
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B143" s="34">
         <v>141</v>
       </c>
       <c r="C143" s="45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D143" s="34">
         <v>141</v>
@@ -5439,13 +5431,13 @@
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B144" s="35">
         <v>142</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D144" s="35">
         <v>142</v>
@@ -5453,13 +5445,13 @@
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B145" s="34">
         <v>143</v>
       </c>
       <c r="C145" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D145" s="34">
         <v>143</v>
@@ -5467,13 +5459,13 @@
     </row>
     <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B146" s="35">
         <v>144</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D146" s="35">
         <v>144</v>
@@ -5481,13 +5473,13 @@
     </row>
     <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B147" s="34">
         <v>145</v>
       </c>
       <c r="C147" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D147" s="34">
         <v>145</v>
@@ -5495,13 +5487,13 @@
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B148" s="35">
         <v>146</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D148" s="35">
         <v>146</v>
@@ -5509,13 +5501,13 @@
     </row>
     <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B149" s="34">
         <v>147</v>
       </c>
       <c r="C149" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D149" s="34">
         <v>147</v>
@@ -5523,13 +5515,13 @@
     </row>
     <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B150" s="35">
         <v>148</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D150" s="35">
         <v>148</v>
@@ -5537,13 +5529,13 @@
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B151" s="34">
         <v>149</v>
       </c>
       <c r="C151" s="45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D151" s="34">
         <v>149</v>
@@ -5551,13 +5543,13 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B152" s="35">
         <v>150</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D152" s="35">
         <v>150</v>
@@ -5565,13 +5557,13 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B153" s="34">
         <v>151</v>
       </c>
       <c r="C153" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D153" s="34">
         <v>151</v>
@@ -5579,13 +5571,13 @@
     </row>
     <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B154" s="35">
         <v>152</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D154" s="35">
         <v>152</v>
@@ -5593,13 +5585,13 @@
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B155" s="34">
         <v>153</v>
       </c>
       <c r="C155" s="45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D155" s="34">
         <v>153</v>
@@ -5607,13 +5599,13 @@
     </row>
     <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B156" s="35">
         <v>154</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D156" s="35">
         <v>154</v>
@@ -5621,13 +5613,13 @@
     </row>
     <row r="157" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B157" s="34">
         <v>155</v>
       </c>
       <c r="C157" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D157" s="34">
         <v>155</v>
@@ -5635,13 +5627,13 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B158" s="35">
         <v>156</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D158" s="35">
         <v>156</v>
@@ -5649,13 +5641,13 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B159" s="34">
         <v>157</v>
       </c>
       <c r="C159" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D159" s="34">
         <v>157</v>
@@ -5663,13 +5655,13 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B160" s="35">
         <v>158</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D160" s="35">
         <v>158</v>
@@ -5677,13 +5669,13 @@
     </row>
     <row r="161" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B161" s="34">
         <v>159</v>
       </c>
       <c r="C161" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D161" s="34">
         <v>159</v>
@@ -5691,13 +5683,13 @@
     </row>
     <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B162" s="35">
         <v>160</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D162" s="35">
         <v>160</v>
@@ -5705,13 +5697,13 @@
     </row>
     <row r="163" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B163" s="34">
         <v>161</v>
       </c>
       <c r="C163" s="45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D163" s="34">
         <v>161</v>
@@ -5719,13 +5711,13 @@
     </row>
     <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B164" s="35">
         <v>162</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D164" s="35">
         <v>162</v>
@@ -5733,13 +5725,13 @@
     </row>
     <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B165" s="34">
         <v>163</v>
       </c>
       <c r="C165" s="45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D165" s="34">
         <v>163</v>
@@ -5747,13 +5739,13 @@
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B166" s="35">
         <v>164</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D166" s="35">
         <v>164</v>
@@ -5761,13 +5753,13 @@
     </row>
     <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B167" s="34">
         <v>165</v>
       </c>
       <c r="C167" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D167" s="34">
         <v>165</v>
@@ -5775,13 +5767,13 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B168" s="35">
         <v>166</v>
       </c>
       <c r="C168" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D168" s="35">
         <v>166</v>
@@ -5789,13 +5781,13 @@
     </row>
     <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B169" s="34">
         <v>167</v>
       </c>
       <c r="C169" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D169" s="34">
         <v>167</v>
@@ -5803,13 +5795,13 @@
     </row>
     <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B170" s="35">
         <v>168</v>
       </c>
       <c r="C170" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D170" s="35">
         <v>168</v>
@@ -5817,13 +5809,13 @@
     </row>
     <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B171" s="34">
         <v>169</v>
       </c>
       <c r="C171" s="45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D171" s="34">
         <v>169</v>
@@ -5831,13 +5823,13 @@
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B172" s="35">
         <v>170</v>
       </c>
       <c r="C172" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D172" s="35">
         <v>170</v>
@@ -5845,13 +5837,13 @@
     </row>
     <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B173" s="34">
         <v>171</v>
       </c>
       <c r="C173" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D173" s="34">
         <v>171</v>
@@ -5859,13 +5851,13 @@
     </row>
     <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B174" s="35">
         <v>172</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D174" s="35">
         <v>172</v>
@@ -5873,13 +5865,13 @@
     </row>
     <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B175" s="34">
         <v>173</v>
       </c>
       <c r="C175" s="45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D175" s="34">
         <v>173</v>
@@ -5887,13 +5879,13 @@
     </row>
     <row r="176" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B176" s="35">
         <v>174</v>
       </c>
       <c r="C176" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D176" s="35">
         <v>174</v>
@@ -5901,13 +5893,13 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B177" s="34">
         <v>175</v>
       </c>
       <c r="C177" s="45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D177" s="34">
         <v>175</v>
@@ -5915,13 +5907,13 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B178" s="35">
         <v>176</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D178" s="35">
         <v>176</v>
@@ -5929,13 +5921,13 @@
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B179" s="34">
         <v>177</v>
       </c>
       <c r="C179" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D179" s="34">
         <v>177</v>
@@ -5943,13 +5935,13 @@
     </row>
     <row r="180" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B180" s="35">
         <v>178</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D180" s="35">
         <v>178</v>
@@ -5957,13 +5949,13 @@
     </row>
     <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B181" s="34">
         <v>179</v>
       </c>
       <c r="C181" s="45" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D181" s="34">
         <v>179</v>
@@ -5971,13 +5963,13 @@
     </row>
     <row r="182" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B182" s="35">
         <v>180</v>
       </c>
       <c r="C182" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D182" s="35">
         <v>180</v>
@@ -5985,13 +5977,13 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B183" s="34">
         <v>181</v>
       </c>
       <c r="C183" s="45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D183" s="34">
         <v>181</v>
@@ -5999,13 +5991,13 @@
     </row>
     <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B184" s="35">
         <v>182</v>
       </c>
       <c r="C184" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D184" s="35">
         <v>182</v>
@@ -6013,13 +6005,13 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B185" s="34">
         <v>183</v>
       </c>
       <c r="C185" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D185" s="34">
         <v>183</v>
@@ -6027,13 +6019,13 @@
     </row>
     <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B186" s="35">
         <v>184</v>
       </c>
       <c r="C186" s="47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D186" s="36">
         <v>184</v>
@@ -6041,13 +6033,13 @@
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B187" s="34">
         <v>185</v>
       </c>
       <c r="C187" s="45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D187" s="34">
         <v>185</v>
@@ -6055,13 +6047,13 @@
     </row>
     <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B188" s="35">
         <v>186</v>
       </c>
       <c r="C188" s="46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D188" s="35">
         <v>186</v>
@@ -6069,13 +6061,13 @@
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B189" s="34">
         <v>187</v>
       </c>
       <c r="C189" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D189" s="34">
         <v>187</v>
@@ -6083,13 +6075,13 @@
     </row>
     <row r="190" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B190" s="35">
         <v>188</v>
       </c>
       <c r="C190" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D190" s="35">
         <v>188</v>
@@ -6097,13 +6089,13 @@
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B191" s="34">
         <v>189</v>
       </c>
       <c r="C191" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D191" s="34">
         <v>189</v>
@@ -6111,13 +6103,13 @@
     </row>
     <row r="192" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B192" s="35">
         <v>190</v>
       </c>
       <c r="C192" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D192" s="35">
         <v>190</v>
@@ -6125,13 +6117,13 @@
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B193" s="34">
         <v>191</v>
       </c>
       <c r="C193" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D193" s="34">
         <v>191</v>
@@ -6139,13 +6131,13 @@
     </row>
     <row r="194" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B194" s="35">
         <v>192</v>
       </c>
       <c r="C194" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D194" s="35">
         <v>192</v>
@@ -6153,13 +6145,13 @@
     </row>
     <row r="195" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B195" s="34">
         <v>193</v>
       </c>
       <c r="C195" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D195" s="34">
         <v>193</v>
@@ -6167,13 +6159,13 @@
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B196" s="35">
         <v>194</v>
       </c>
       <c r="C196" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D196" s="35">
         <v>194</v>
@@ -6181,13 +6173,13 @@
     </row>
     <row r="197" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B197" s="34">
         <v>195</v>
       </c>
       <c r="C197" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D197" s="34">
         <v>195</v>
@@ -6195,13 +6187,13 @@
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B198" s="35">
         <v>196</v>
       </c>
       <c r="C198" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D198" s="35">
         <v>196</v>
@@ -6209,13 +6201,13 @@
     </row>
     <row r="199" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B199" s="34">
         <v>197</v>
       </c>
       <c r="C199" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D199" s="34">
         <v>197</v>
@@ -6223,13 +6215,13 @@
     </row>
     <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B200" s="35">
         <v>198</v>
       </c>
       <c r="C200" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D200" s="35">
         <v>198</v>
@@ -6237,13 +6229,13 @@
     </row>
     <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B201" s="34">
         <v>199</v>
       </c>
       <c r="C201" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D201" s="34">
         <v>199</v>
@@ -6251,13 +6243,13 @@
     </row>
     <row r="202" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="47" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B202" s="36">
         <v>200</v>
       </c>
       <c r="C202" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D202" s="35">
         <v>200</v>

</xml_diff>

<commit_message>
970806 - +1783 Free basket
ریسک زیاد و نداشتن استراتژی برای خرید
ضرر 1 میلیون تومان
همه سبد بدون استراتژی اولیه خریده شده بود لذا در بدترین وضعیت خریداری شده بود
و تمامی در حال ریزش هستند یعنی در بالاترین قیمت خریداری شده بودند
به همین خاطر سبد خالی شد
</commit_message>
<xml_diff>
--- a/Sellbuy.xlsx
+++ b/Sellbuy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FBADF3-B346-408D-9584-F4EE8A5D80EB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B13F36F-8138-49AA-B743-929F301E8545}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1230,7 +1230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1280,12 +1280,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1302,9 +1296,6 @@
     <xf numFmtId="3" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="37" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1361,18 +1352,21 @@
     <xf numFmtId="49" fontId="8" fillId="10" borderId="14" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1431,12 +1425,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1786,43 +1774,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="E2" s="51" t="s">
+      <c r="C2" s="48"/>
+      <c r="E2" s="47" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-      <c r="I2" s="52" t="s">
+      <c r="G2" s="48"/>
+      <c r="I2" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="53"/>
+      <c r="L2" s="51"/>
     </row>
     <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="65">
         <f>SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&gt;0",Sheet3!K3:K18,"&gt;0")</f>
-        <v>2154427.2533821166</v>
-      </c>
-      <c r="G3" s="68"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="55"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="66"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1834,23 +1822,23 @@
       <c r="C4" s="2">
         <v>140000000</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="65">
+      <c r="F4" s="63">
         <f>ABS(SUMIFS(Sheet3!J3:J18,Sheet3!J3:J18,"&lt;0",Sheet3!K3:K18,"&gt;0"))</f>
-        <v>14583245.679744273</v>
-      </c>
-      <c r="G4" s="66"/>
-      <c r="I4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="64"/>
+      <c r="I4" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63">
+      <c r="J4" s="61"/>
+      <c r="K4" s="61">
         <f>DATEDIF(Sheet2!B4,F7,"d")-1</f>
         <v>39</v>
       </c>
-      <c r="L4" s="64"/>
+      <c r="L4" s="62"/>
     </row>
     <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
@@ -1862,24 +1850,24 @@
       <c r="C5" s="2">
         <v>10000000</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="69">
+      <c r="F5" s="67">
         <f>F3-F4</f>
-        <v>-12428818.426362157</v>
-      </c>
-      <c r="G5" s="70"/>
-      <c r="I5" s="56">
+        <v>0</v>
+      </c>
+      <c r="G5" s="68"/>
+      <c r="I5" s="54" t="e">
         <f>((C14*100)/C13)-100</f>
-        <v>-4.9460428960216234</v>
-      </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="56">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="55"/>
+      <c r="K5" s="54">
         <f>((C14*100)/C12)-100</f>
-        <v>-4.3784890221603092</v>
-      </c>
-      <c r="L5" s="57"/>
+        <v>-100</v>
+      </c>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
@@ -1891,10 +1879,10 @@
       <c r="C6" s="2">
         <v>30000000</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="59"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -1906,181 +1894,174 @@
       <c r="C7" s="2">
         <v>70000000</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="36" t="s">
         <v>289</v>
       </c>
-      <c r="F7" s="71">
+      <c r="F7" s="69">
         <v>35647</v>
       </c>
-      <c r="G7" s="71"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="61"/>
+      <c r="G7" s="69"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="59"/>
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="4">
         <f>SUMIFS(Sheet3!J3:J18,Sheet3!K3:K18,"=0",Sheet3!J3:J18,"&gt;0")</f>
-        <v>26800150.399080981</v>
+        <v>30431665.58401214</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="4">
         <f>ABS(SUMIFS(Sheet3!J3:J18,Sheet3!K3:K18,"=0",Sheet3!J3:J18,"&lt;0"))</f>
-        <v>24459596.960380837</v>
-      </c>
-      <c r="E9" s="51" t="s">
+        <v>40155861.997232981</v>
+      </c>
+      <c r="E9" s="47" t="s">
         <v>279</v>
       </c>
       <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
-      <c r="I9" s="51" t="s">
+      <c r="G9" s="48"/>
+      <c r="I9" s="47" t="s">
         <v>282</v>
       </c>
       <c r="J9" s="49"/>
       <c r="K9" s="49"/>
-      <c r="L9" s="50"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="4">
         <f>SUM(C4:C7)</f>
         <v>250000000</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="29" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="47" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="50"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="4">
         <v>27400000</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="34">
         <v>410</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="34">
         <v>770</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="34">
         <f>((F11*100)/E11)-100</f>
         <v>87.804878048780495</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="34">
         <v>410</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="34">
         <v>770</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="34">
         <v>380</v>
       </c>
-      <c r="L11" s="37">
+      <c r="L11" s="34">
         <f>(J11-I11)/(I11-K11)</f>
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="50"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="4">
         <f>SUM(C10,(C8-C9))-C11</f>
-        <v>224940553.43870014</v>
+        <v>212875803.58677915</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="26">
+      <c r="B13" s="46"/>
+      <c r="C13" s="24">
         <f>Sheet2!G19</f>
-        <v>226283642</v>
-      </c>
-      <c r="E13" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="47" t="s">
         <v>286</v>
       </c>
       <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A14" s="72" t="s">
+      <c r="A14" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="26">
+      <c r="B14" s="46"/>
+      <c r="C14" s="24">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet3!E3:E18)</f>
-        <v>215091556</v>
-      </c>
-      <c r="E14" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="29" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="A15" s="72"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="26"/>
-      <c r="E15" s="38" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="24"/>
+      <c r="E15" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="F15" s="37" t="b">
+      <c r="F15" s="34" t="b">
         <f>ISNUMBER(SEARCH(E15,Sheet4!A:A))</f>
         <v>0</v>
       </c>
-      <c r="G15" s="37" t="b">
+      <c r="G15" s="34" t="b">
         <f>COUNTIF(Sheet4!C:C,"*"&amp;Sheet1!E15&amp;"*")&gt;0</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:L9"/>
@@ -2097,6 +2078,13 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2108,7 +2096,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,17 +2113,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
@@ -2190,7 +2178,7 @@
         <f>F3*C3</f>
         <v>39997734</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="22">
         <f>IF(Sheet3!K3,(G3*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2224,7 +2212,7 @@
         <f>F4*C4</f>
         <v>70068801</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="22">
         <f>IF(Sheet3!K4,(G4*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2257,7 +2245,7 @@
         <f t="shared" ref="G5:G16" si="2">F5*C5</f>
         <v>29991996</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="22">
         <f>IF(Sheet3!K5,(G5*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2290,7 +2278,7 @@
         <f t="shared" si="2"/>
         <v>29997520</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="22">
         <f>IF(Sheet3!K6,(G6*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2323,7 +2311,7 @@
         <f t="shared" si="2"/>
         <v>9997632</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="22">
         <f>IF(Sheet3!K7,(G7*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2356,7 +2344,7 @@
         <f t="shared" si="2"/>
         <v>29997676</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="22">
         <f>IF(Sheet3!K8,(G8*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2389,7 +2377,7 @@
         <f t="shared" si="2"/>
         <v>42285294</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="22">
         <f>IF(Sheet3!K9,(G9*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2422,7 +2410,7 @@
         <f t="shared" si="2"/>
         <v>14990206</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="22">
         <f>IF(Sheet3!K10,(G10*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2455,7 +2443,7 @@
         <f t="shared" si="2"/>
         <v>50002806</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="22">
         <f>IF(Sheet3!K11,(G11*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2488,7 +2476,7 @@
         <f t="shared" si="2"/>
         <v>10298934</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="22">
         <f>IF(Sheet3!K12,(G12*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2521,7 +2509,7 @@
         <f t="shared" si="2"/>
         <v>26902351</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="22">
         <f>IF(Sheet3!K13,(G13*100)/G19,0)</f>
         <v>0</v>
       </c>
@@ -2540,14 +2528,14 @@
       <c r="C14" s="6">
         <v>9288</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="37">
         <v>10716</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="37">
         <f t="shared" si="0"/>
         <v>99530208</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="37">
         <v>10766</v>
       </c>
       <c r="G14" s="17">
@@ -2556,7 +2544,7 @@
       </c>
       <c r="H14" s="11">
         <f>IF(Sheet3!K14,(G14*100)/G19,0)</f>
-        <v>44.189941047528308</v>
+        <v>0</v>
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
@@ -2573,14 +2561,14 @@
       <c r="C15" s="6">
         <v>33014</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="37">
         <v>2300</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="37">
         <f t="shared" si="0"/>
         <v>75932200</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="37">
         <v>2311</v>
       </c>
       <c r="G15" s="17">
@@ -2589,7 +2577,7 @@
       </c>
       <c r="H15" s="11">
         <f>IF(Sheet3!K15,(G15*100)/G19,0)</f>
-        <v>33.716689958525592</v>
+        <v>0</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
@@ -2600,20 +2588,20 @@
       <c r="A16" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="39">
         <v>35629</v>
       </c>
       <c r="C16" s="6">
         <v>3480</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="38">
         <v>14300</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="38">
         <f t="shared" si="0"/>
         <v>49764000</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="38">
         <v>14366</v>
       </c>
       <c r="G16" s="17">
@@ -2622,9 +2610,9 @@
       </c>
       <c r="H16" s="11">
         <f>IF(Sheet3!K16,(G16*100)/G19,0)</f>
-        <v>22.093368993946104</v>
-      </c>
-      <c r="I16" s="41">
+        <v>0</v>
+      </c>
+      <c r="I16" s="38">
         <f t="shared" si="1"/>
         <v>13647.7</v>
       </c>
@@ -2634,7 +2622,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="29">
+      <c r="E17" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2654,7 +2642,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="29">
+      <c r="E18" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2670,21 +2658,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.45">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="76"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="17">
         <f>SUMIF(Sheet3!K3:K18,"&gt;0",Sheet2!G3:G18)</f>
-        <v>226283642</v>
+        <v>0</v>
       </c>
       <c r="H19" s="17">
         <f>SUM(H4:H18)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2721,21 +2709,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="82" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
@@ -2797,15 +2785,15 @@
         <f>E3-F3</f>
         <v>45303110.000353366</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="21">
         <f>DATEDIF(Sheet2!B3,B3,"d")</f>
         <v>11</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="28">
         <f>((G3*100)/Sheet2!G3)-100</f>
         <v>13.264191417327197</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="23">
         <f>Sheet3!G3-Sheet2!G3</f>
         <v>5305376.0003533661</v>
       </c>
@@ -2839,15 +2827,15 @@
         <f t="shared" ref="G4:G12" si="2">E4-F4</f>
         <v>84300317.330177292</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="21">
         <f>DATEDIF(Sheet2!B4,B4,"d")</f>
         <v>19</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="22">
         <f>((G4*100)/Sheet2!G4)-100</f>
         <v>20.310774734360436</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="23">
         <f>Sheet3!G4-Sheet2!G4</f>
         <v>14231516.330177292</v>
       </c>
@@ -2881,15 +2869,15 @@
         <f t="shared" si="2"/>
         <v>30342985.100908022</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <f>DATEDIF(Sheet2!B5,B5,"d")</f>
         <v>20</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="22">
         <f>((G5*100)/Sheet2!G5)-100</f>
         <v>1.1702758993033342</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="23">
         <f>Sheet3!G5-Sheet2!G5</f>
         <v>350989.10090802237</v>
       </c>
@@ -2923,15 +2911,15 @@
         <f t="shared" si="2"/>
         <v>36909788.9676423</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="21">
         <f>DATEDIF(Sheet2!B6,B6,"d")</f>
         <v>19</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="22">
         <f>((G6*100)/Sheet2!G6)-100</f>
         <v>23.042801430392572</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="23">
         <f>Sheet3!G6-Sheet2!G6</f>
         <v>6912268.9676422998</v>
       </c>
@@ -2965,15 +2953,15 @@
         <f t="shared" si="2"/>
         <v>9935279.8131133504</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <f>DATEDIF(Sheet2!B7,B7,"d")</f>
         <v>17</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="22">
         <f>((G7*100)/Sheet2!G7)-100</f>
         <v>-0.62366955381683908</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="23">
         <f>Sheet3!G7-Sheet2!G7</f>
         <v>-62352.186886649579</v>
       </c>
@@ -3007,15 +2995,15 @@
         <f t="shared" si="2"/>
         <v>26896966.586817309</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="21">
         <f>DATEDIF(Sheet2!B8,B8,"d")</f>
         <v>4</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="22">
         <f>((G8*100)/Sheet2!G8)-100</f>
         <v>-10.336498778047641</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="23">
         <f>Sheet3!G8-Sheet2!G8</f>
         <v>-3100709.4131826907</v>
       </c>
@@ -3049,15 +3037,15 @@
         <f t="shared" si="2"/>
         <v>34663737.985307172</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <f>DATEDIF(Sheet2!B9,B9,"d")</f>
         <v>11</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="22">
         <f>((G9*100)/Sheet2!G9)-100</f>
         <v>-18.024129179976441</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="23">
         <f>Sheet3!G9-Sheet2!G9</f>
         <v>-7621556.0146928281</v>
       </c>
@@ -3091,15 +3079,15 @@
         <f t="shared" si="2"/>
         <v>12989011.937704436</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="21">
         <f>DATEDIF(Sheet2!B10,B10,"d")</f>
         <v>7</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="22">
         <f>((G10*100)/Sheet2!G10)-100</f>
         <v>-13.35001041543768</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="23">
         <f>Sheet3!G10-Sheet2!G10</f>
         <v>-2001194.0622955635</v>
       </c>
@@ -3133,15 +3121,15 @@
         <f t="shared" si="2"/>
         <v>39551094.176337965</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="21">
         <f>DATEDIF(Sheet2!B11,B11,"d")</f>
         <v>8</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="22">
         <f>((G11*100)/Sheet2!G11)-100</f>
         <v>-20.90225061301966</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="23">
         <f>Sheet3!G11-Sheet2!G11</f>
         <v>-10451711.823662035</v>
       </c>
@@ -3167,7 +3155,7 @@
         <f t="shared" si="0"/>
         <v>9401340</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="27">
         <f t="shared" si="1"/>
         <v>54055.780921755599</v>
       </c>
@@ -3175,15 +3163,15 @@
         <f t="shared" si="2"/>
         <v>9347284.2190782446</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <f>DATEDIF(Sheet2!B12,B12,"d")</f>
         <v>5</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="22">
         <f>((G12*100)/Sheet2!G12)-100</f>
         <v>-9.2402745849400958</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="23">
         <f>Sheet3!G12-Sheet2!G12</f>
         <v>-951649.78092175536</v>
       </c>
@@ -3217,15 +3205,15 @@
         <f>E13-F13</f>
         <v>26631927.321260683</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="21">
         <f>DATEDIF(Sheet2!B13,B13,"d")</f>
         <v>2</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="22">
         <f>((G13*100)/Sheet2!G13)-100</f>
         <v>-1.0052046333769056</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="23">
         <f>Sheet3!G13-Sheet2!G13</f>
         <v>-270423.67873931676</v>
       </c>
@@ -3234,128 +3222,128 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="42">
-        <v>35647</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B14" s="14">
+        <v>35648</v>
+      </c>
+      <c r="C14" s="13">
         <f>Sheet2!C14</f>
         <v>9288</v>
       </c>
-      <c r="D14" s="40">
-        <v>9502</v>
-      </c>
-      <c r="E14" s="40">
+      <c r="D14" s="15">
+        <v>9350</v>
+      </c>
+      <c r="E14" s="15">
         <f t="shared" si="0"/>
-        <v>88254576</v>
-      </c>
-      <c r="F14" s="40">
+        <v>86842800</v>
+      </c>
+      <c r="F14" s="15">
         <f t="shared" si="1"/>
-        <v>507445.7498184758</v>
-      </c>
-      <c r="G14" s="40">
+        <v>499328.32675255201</v>
+      </c>
+      <c r="G14" s="15">
         <f t="shared" ref="G14:G16" si="3">E14-F14</f>
-        <v>87747130.250181526</v>
-      </c>
-      <c r="H14" s="19">
+        <v>86343471.673247442</v>
+      </c>
+      <c r="H14" s="21">
         <f>DATEDIF(Sheet2!B14,B14,"d")-1</f>
-        <v>18</v>
-      </c>
-      <c r="I14" s="24">
+        <v>19</v>
+      </c>
+      <c r="I14" s="22">
         <f>((G14*100)/Sheet2!G14)-100</f>
-        <v>-12.248138169428572</v>
-      </c>
-      <c r="J14" s="20">
+        <v>-13.651872435714296</v>
+      </c>
+      <c r="J14" s="23">
         <f>Sheet3!G14-Sheet2!G14</f>
-        <v>-12247477.749818474</v>
-      </c>
-      <c r="K14" s="27">
-        <v>1</v>
+        <v>-13651136.326752558</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="48">
-        <v>35647</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="B15" s="14">
+        <v>35648</v>
+      </c>
+      <c r="C15" s="13">
         <f>Sheet2!C15</f>
         <v>33014</v>
       </c>
-      <c r="D15" s="40">
-        <v>2390</v>
-      </c>
-      <c r="E15" s="40">
+      <c r="D15" s="15">
+        <v>2435</v>
+      </c>
+      <c r="E15" s="15">
         <f t="shared" si="0"/>
-        <v>78903460</v>
-      </c>
-      <c r="F15" s="40">
+        <v>80389090</v>
+      </c>
+      <c r="F15" s="15">
         <f t="shared" si="1"/>
-        <v>453678.7466178764</v>
-      </c>
-      <c r="G15" s="40">
+        <v>462220.81506884057</v>
+      </c>
+      <c r="G15" s="15">
         <f t="shared" si="3"/>
-        <v>78449781.253382117</v>
-      </c>
-      <c r="H15" s="19">
+        <v>79926869.184931159</v>
+      </c>
+      <c r="H15" s="21">
         <f>DATEDIF(Sheet2!B15,B15,"d")-1</f>
+        <v>19</v>
+      </c>
+      <c r="I15" s="22">
+        <f>((G15*100)/Sheet2!G15)-100</f>
+        <v>4.7598116982734808</v>
+      </c>
+      <c r="J15" s="23">
+        <f>Sheet3!G15-Sheet2!G15</f>
+        <v>3631515.184931159</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16" s="14">
+        <v>35648</v>
+      </c>
+      <c r="C16" s="13">
+        <v>3480</v>
+      </c>
+      <c r="D16" s="15">
+        <v>13858</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="0"/>
+        <v>48225840</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="1"/>
+        <v>277288.71009958559</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="3"/>
+        <v>47948551.289900415</v>
+      </c>
+      <c r="H16" s="21">
+        <f>DATEDIF(Sheet2!B16,B16,"d")-1</f>
         <v>18</v>
       </c>
-      <c r="I15" s="24">
-        <f>((G15*100)/Sheet2!G15)-100</f>
-        <v>2.8237987510774474</v>
-      </c>
-      <c r="J15" s="20">
-        <f>Sheet3!G15-Sheet2!G15</f>
-        <v>2154427.2533821166</v>
-      </c>
-      <c r="K15" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="B16" s="48">
-        <v>35647</v>
-      </c>
-      <c r="C16" s="6">
-        <v>3480</v>
-      </c>
-      <c r="D16" s="41">
-        <v>13774</v>
-      </c>
-      <c r="E16" s="41">
-        <f t="shared" si="0"/>
-        <v>47933520</v>
-      </c>
-      <c r="F16" s="41">
-        <f t="shared" si="1"/>
-        <v>275607.92992579681</v>
-      </c>
-      <c r="G16" s="41">
-        <f t="shared" si="3"/>
-        <v>47657912.070074201</v>
-      </c>
-      <c r="H16" s="19">
-        <f>DATEDIF(Sheet2!B16,B16,"d")-1</f>
-        <v>17</v>
-      </c>
-      <c r="I16" s="24">
+      <c r="I16" s="22">
         <f>((G16*100)/Sheet2!G16)-100</f>
-        <v>-4.6721264166306753</v>
-      </c>
-      <c r="J16" s="20">
+        <v>-4.0907744940952142</v>
+      </c>
+      <c r="J16" s="23">
         <f>Sheet3!G16-Sheet2!G16</f>
-        <v>-2335767.9299257994</v>
-      </c>
-      <c r="K16" s="17">
-        <v>1</v>
+        <v>-2045128.7100995854</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -3366,10 +3354,10 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="28"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="6"/>
@@ -3379,28 +3367,28 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="28"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="25"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="84">
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="80">
         <f>SUMIF(K3:K18,"&gt;0",G3:G18)</f>
-        <v>213854823.57363784</v>
-      </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3429,2829 +3417,2829 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.28515625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="58.85546875" style="43" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="31">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="32">
         <v>2</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="32">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="31">
         <v>3</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="31">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="32">
         <v>4</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="31">
         <v>5</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="32">
         <v>6</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="32">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="31">
         <v>7</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="32">
         <v>8</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="32">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="31">
         <v>9</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="31">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="32">
         <v>10</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="32">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="31">
         <v>11</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="31">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="32">
         <v>12</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="31">
         <v>13</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="31">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="32">
         <v>14</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="32">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="31">
         <v>15</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="31">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18" s="32">
         <v>16</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="32">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="31">
         <v>17</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="31">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="32">
         <v>18</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="32">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="31">
         <v>19</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="31">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="32">
         <v>20</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="32">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="31">
         <v>21</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="31">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="32">
         <v>22</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="32">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="31">
         <v>23</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="31">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26" s="32">
         <v>24</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="32">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B27" s="31">
         <v>25</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="31">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="35">
+      <c r="B28" s="32">
         <v>26</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="32">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="31">
         <v>27</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="31">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="32">
         <v>28</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="32">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="31">
         <v>29</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="31">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="35">
+      <c r="B32" s="32">
         <v>30</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="35">
+      <c r="D32" s="32">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="31">
         <v>31</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="31">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="35">
+      <c r="B34" s="32">
         <v>32</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="D34" s="35">
+      <c r="D34" s="32">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="34">
+      <c r="B35" s="31">
         <v>33</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="31">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B36" s="32">
         <v>34</v>
       </c>
-      <c r="C36" s="46" t="s">
+      <c r="C36" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="35">
+      <c r="D36" s="32">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="34">
+      <c r="B37" s="31">
         <v>35</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="31">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="35">
+      <c r="B38" s="32">
         <v>36</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="35">
+      <c r="D38" s="32">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="34">
+      <c r="B39" s="31">
         <v>37</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="31">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="35">
+      <c r="B40" s="32">
         <v>38</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="35">
+      <c r="D40" s="32">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="34">
+      <c r="B41" s="31">
         <v>39</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="31">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="35">
+      <c r="B42" s="32">
         <v>40</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="35">
+      <c r="D42" s="32">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="34">
+      <c r="B43" s="31">
         <v>41</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="31">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="35">
+      <c r="B44" s="32">
         <v>42</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="35">
+      <c r="D44" s="32">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="34">
+      <c r="B45" s="31">
         <v>43</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="34">
+      <c r="D45" s="31">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="35">
+      <c r="B46" s="32">
         <v>44</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="35">
+      <c r="D46" s="32">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="34">
+      <c r="B47" s="31">
         <v>45</v>
       </c>
-      <c r="C47" s="45" t="s">
+      <c r="C47" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="34">
+      <c r="D47" s="31">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="46" t="s">
+      <c r="A48" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="35">
+      <c r="B48" s="32">
         <v>46</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="35">
+      <c r="D48" s="32">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="34">
+      <c r="B49" s="31">
         <v>47</v>
       </c>
-      <c r="C49" s="45" t="s">
+      <c r="C49" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="34">
+      <c r="D49" s="31">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="35">
+      <c r="B50" s="32">
         <v>48</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C50" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="D50" s="35">
+      <c r="D50" s="32">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="34">
+      <c r="B51" s="31">
         <v>49</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="34">
+      <c r="D51" s="31">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="35">
+      <c r="B52" s="32">
         <v>50</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C52" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="35">
+      <c r="D52" s="32">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="34">
+      <c r="B53" s="31">
         <v>51</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="34">
+      <c r="D53" s="31">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="35">
+      <c r="B54" s="32">
         <v>52</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="D54" s="35">
+      <c r="D54" s="32">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="34">
+      <c r="B55" s="31">
         <v>53</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="34">
+      <c r="D55" s="31">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="35">
+      <c r="B56" s="32">
         <v>54</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D56" s="35">
+      <c r="D56" s="32">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="34">
+      <c r="B57" s="31">
         <v>55</v>
       </c>
-      <c r="C57" s="45" t="s">
+      <c r="C57" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="34">
+      <c r="D57" s="31">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="35">
+      <c r="B58" s="32">
         <v>56</v>
       </c>
-      <c r="C58" s="46" t="s">
+      <c r="C58" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="35">
+      <c r="D58" s="32">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B59" s="34">
+      <c r="B59" s="31">
         <v>57</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C59" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="34">
+      <c r="D59" s="31">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="35">
+      <c r="B60" s="32">
         <v>58</v>
       </c>
-      <c r="C60" s="46" t="s">
+      <c r="C60" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="D60" s="35">
+      <c r="D60" s="32">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="45" t="s">
+      <c r="A61" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="34">
+      <c r="B61" s="31">
         <v>59</v>
       </c>
-      <c r="C61" s="45" t="s">
+      <c r="C61" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="D61" s="34">
+      <c r="D61" s="31">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="35">
+      <c r="B62" s="32">
         <v>60</v>
       </c>
-      <c r="C62" s="46" t="s">
+      <c r="C62" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="D62" s="35">
+      <c r="D62" s="32">
         <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="34">
+      <c r="B63" s="31">
         <v>61</v>
       </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="D63" s="34">
+      <c r="D63" s="31">
         <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="46" t="s">
+      <c r="A64" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B64" s="35">
+      <c r="B64" s="32">
         <v>62</v>
       </c>
-      <c r="C64" s="46" t="s">
+      <c r="C64" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="35">
+      <c r="D64" s="32">
         <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45" t="s">
+      <c r="A65" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="34">
+      <c r="B65" s="31">
         <v>63</v>
       </c>
-      <c r="C65" s="45" t="s">
+      <c r="C65" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="34">
+      <c r="D65" s="31">
         <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="46" t="s">
+      <c r="A66" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B66" s="35">
+      <c r="B66" s="32">
         <v>64</v>
       </c>
-      <c r="C66" s="46" t="s">
+      <c r="C66" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D66" s="35">
+      <c r="D66" s="32">
         <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="45" t="s">
+      <c r="A67" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="34">
+      <c r="B67" s="31">
         <v>65</v>
       </c>
-      <c r="C67" s="45" t="s">
+      <c r="C67" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="D67" s="34">
+      <c r="D67" s="31">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="35">
+      <c r="B68" s="32">
         <v>66</v>
       </c>
-      <c r="C68" s="46" t="s">
+      <c r="C68" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="35">
+      <c r="D68" s="32">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="45" t="s">
+      <c r="A69" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="34">
+      <c r="B69" s="31">
         <v>67</v>
       </c>
-      <c r="C69" s="45" t="s">
+      <c r="C69" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D69" s="34">
+      <c r="D69" s="31">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="46" t="s">
+      <c r="A70" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B70" s="35">
+      <c r="B70" s="32">
         <v>68</v>
       </c>
-      <c r="C70" s="46" t="s">
+      <c r="C70" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D70" s="35">
+      <c r="D70" s="32">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="45" t="s">
+      <c r="A71" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="34">
+      <c r="B71" s="31">
         <v>69</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="D71" s="34">
+      <c r="D71" s="31">
         <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="46" t="s">
+      <c r="A72" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="35">
+      <c r="B72" s="32">
         <v>70</v>
       </c>
-      <c r="C72" s="46" t="s">
+      <c r="C72" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D72" s="35">
+      <c r="D72" s="32">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="45" t="s">
+      <c r="A73" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="34">
+      <c r="B73" s="31">
         <v>71</v>
       </c>
-      <c r="C73" s="45" t="s">
+      <c r="C73" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="34">
+      <c r="D73" s="31">
         <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="46" t="s">
+      <c r="A74" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="B74" s="35">
+      <c r="B74" s="32">
         <v>72</v>
       </c>
-      <c r="C74" s="46" t="s">
+      <c r="C74" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="D74" s="35">
+      <c r="D74" s="32">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="34">
+      <c r="B75" s="31">
         <v>73</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="C75" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="34">
+      <c r="D75" s="31">
         <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="46" t="s">
+      <c r="A76" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="35">
+      <c r="B76" s="32">
         <v>74</v>
       </c>
-      <c r="C76" s="46" t="s">
+      <c r="C76" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="D76" s="35">
+      <c r="D76" s="32">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="45" t="s">
+      <c r="A77" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="34">
+      <c r="B77" s="31">
         <v>75</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C77" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="D77" s="34">
+      <c r="D77" s="31">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="46" t="s">
+      <c r="A78" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="35">
+      <c r="B78" s="32">
         <v>76</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="C78" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="D78" s="35">
+      <c r="D78" s="32">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="45" t="s">
+      <c r="A79" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B79" s="34">
+      <c r="B79" s="31">
         <v>77</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="C79" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="D79" s="34">
+      <c r="D79" s="31">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="46" t="s">
+      <c r="A80" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="B80" s="35">
+      <c r="B80" s="32">
         <v>78</v>
       </c>
-      <c r="C80" s="46" t="s">
+      <c r="C80" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="D80" s="35">
+      <c r="D80" s="32">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="45" t="s">
+      <c r="A81" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="34">
+      <c r="B81" s="31">
         <v>79</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="D81" s="34">
+      <c r="D81" s="31">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="46" t="s">
+      <c r="A82" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="35">
+      <c r="B82" s="32">
         <v>80</v>
       </c>
-      <c r="C82" s="46" t="s">
+      <c r="C82" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="D82" s="35">
+      <c r="D82" s="32">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="45" t="s">
+      <c r="A83" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="34">
+      <c r="B83" s="31">
         <v>81</v>
       </c>
-      <c r="C83" s="45" t="s">
+      <c r="C83" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D83" s="34">
+      <c r="D83" s="31">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="46" t="s">
+      <c r="A84" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B84" s="35">
+      <c r="B84" s="32">
         <v>82</v>
       </c>
-      <c r="C84" s="46" t="s">
+      <c r="C84" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="D84" s="35">
+      <c r="D84" s="32">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="45" t="s">
+      <c r="A85" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="B85" s="34">
+      <c r="B85" s="31">
         <v>83</v>
       </c>
-      <c r="C85" s="45" t="s">
+      <c r="C85" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="D85" s="34">
+      <c r="D85" s="31">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="46" t="s">
+      <c r="A86" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B86" s="35">
+      <c r="B86" s="32">
         <v>84</v>
       </c>
-      <c r="C86" s="46" t="s">
+      <c r="C86" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="D86" s="35">
+      <c r="D86" s="32">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="45" t="s">
+      <c r="A87" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="B87" s="34">
+      <c r="B87" s="31">
         <v>85</v>
       </c>
-      <c r="C87" s="45" t="s">
+      <c r="C87" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="D87" s="34">
+      <c r="D87" s="31">
         <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="46" t="s">
+      <c r="A88" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="B88" s="35">
+      <c r="B88" s="32">
         <v>86</v>
       </c>
-      <c r="C88" s="46" t="s">
+      <c r="C88" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="D88" s="35">
+      <c r="D88" s="32">
         <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="45" t="s">
+      <c r="A89" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="B89" s="34">
+      <c r="B89" s="31">
         <v>87</v>
       </c>
-      <c r="C89" s="45" t="s">
+      <c r="C89" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="D89" s="34">
+      <c r="D89" s="31">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="46" t="s">
+      <c r="A90" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="B90" s="35">
+      <c r="B90" s="32">
         <v>88</v>
       </c>
-      <c r="C90" s="46" t="s">
+      <c r="C90" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="D90" s="35">
+      <c r="D90" s="32">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="45" t="s">
+      <c r="A91" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="B91" s="34">
+      <c r="B91" s="31">
         <v>89</v>
       </c>
-      <c r="C91" s="45" t="s">
+      <c r="C91" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="D91" s="34">
+      <c r="D91" s="31">
         <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="46" t="s">
+      <c r="A92" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B92" s="35">
+      <c r="B92" s="32">
         <v>90</v>
       </c>
-      <c r="C92" s="46" t="s">
+      <c r="C92" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="D92" s="35">
+      <c r="D92" s="32">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="45" t="s">
+      <c r="A93" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="B93" s="34">
+      <c r="B93" s="31">
         <v>91</v>
       </c>
-      <c r="C93" s="45" t="s">
+      <c r="C93" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D93" s="34">
+      <c r="D93" s="31">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="46" t="s">
+      <c r="A94" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="B94" s="35">
+      <c r="B94" s="32">
         <v>92</v>
       </c>
-      <c r="C94" s="46" t="s">
+      <c r="C94" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="D94" s="35">
+      <c r="D94" s="32">
         <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="45" t="s">
+      <c r="A95" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="B95" s="34">
+      <c r="B95" s="31">
         <v>93</v>
       </c>
-      <c r="C95" s="45" t="s">
+      <c r="C95" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D95" s="34">
+      <c r="D95" s="31">
         <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="46" t="s">
+      <c r="A96" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="B96" s="35">
+      <c r="B96" s="32">
         <v>94</v>
       </c>
-      <c r="C96" s="46" t="s">
+      <c r="C96" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D96" s="35">
+      <c r="D96" s="32">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="45" t="s">
+      <c r="A97" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B97" s="34">
+      <c r="B97" s="31">
         <v>95</v>
       </c>
-      <c r="C97" s="45" t="s">
+      <c r="C97" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="D97" s="34">
+      <c r="D97" s="31">
         <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="46" t="s">
+      <c r="A98" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="B98" s="35">
+      <c r="B98" s="32">
         <v>96</v>
       </c>
-      <c r="C98" s="46" t="s">
+      <c r="C98" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="D98" s="35">
+      <c r="D98" s="32">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="45" t="s">
+      <c r="A99" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="B99" s="34">
+      <c r="B99" s="31">
         <v>97</v>
       </c>
-      <c r="C99" s="45" t="s">
+      <c r="C99" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="D99" s="34">
+      <c r="D99" s="31">
         <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="46" t="s">
+      <c r="A100" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="35">
+      <c r="B100" s="32">
         <v>98</v>
       </c>
-      <c r="C100" s="46" t="s">
+      <c r="C100" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="D100" s="35">
+      <c r="D100" s="32">
         <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="45" t="s">
+      <c r="A101" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="B101" s="34">
+      <c r="B101" s="31">
         <v>99</v>
       </c>
-      <c r="C101" s="45" t="s">
+      <c r="C101" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="D101" s="34">
+      <c r="D101" s="31">
         <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="46" t="s">
+      <c r="A102" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="B102" s="35">
+      <c r="B102" s="32">
         <v>100</v>
       </c>
-      <c r="C102" s="46" t="s">
+      <c r="C102" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="D102" s="35">
+      <c r="D102" s="32">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="45" t="s">
+      <c r="A103" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B103" s="34">
+      <c r="B103" s="31">
         <v>101</v>
       </c>
-      <c r="C103" s="45" t="s">
+      <c r="C103" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="D103" s="34">
+      <c r="D103" s="31">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="46" t="s">
+      <c r="A104" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B104" s="35">
+      <c r="B104" s="32">
         <v>102</v>
       </c>
-      <c r="C104" s="46" t="s">
+      <c r="C104" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="D104" s="35">
+      <c r="D104" s="32">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="45" t="s">
+      <c r="A105" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="B105" s="34">
+      <c r="B105" s="31">
         <v>103</v>
       </c>
-      <c r="C105" s="45" t="s">
+      <c r="C105" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="D105" s="34">
+      <c r="D105" s="31">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="46" t="s">
+      <c r="A106" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="B106" s="35">
+      <c r="B106" s="32">
         <v>104</v>
       </c>
-      <c r="C106" s="46" t="s">
+      <c r="C106" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="D106" s="35">
+      <c r="D106" s="32">
         <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="45" t="s">
+      <c r="A107" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="B107" s="34">
+      <c r="B107" s="31">
         <v>105</v>
       </c>
-      <c r="C107" s="45" t="s">
+      <c r="C107" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="D107" s="34">
+      <c r="D107" s="31">
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="46" t="s">
+      <c r="A108" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="B108" s="35">
+      <c r="B108" s="32">
         <v>106</v>
       </c>
-      <c r="C108" s="46" t="s">
+      <c r="C108" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="D108" s="35">
+      <c r="D108" s="32">
         <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="45" t="s">
+      <c r="A109" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="B109" s="34">
+      <c r="B109" s="31">
         <v>107</v>
       </c>
-      <c r="C109" s="45" t="s">
+      <c r="C109" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="D109" s="34">
+      <c r="D109" s="31">
         <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="46" t="s">
+      <c r="A110" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="B110" s="35">
+      <c r="B110" s="32">
         <v>108</v>
       </c>
-      <c r="C110" s="46" t="s">
+      <c r="C110" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="D110" s="35">
+      <c r="D110" s="32">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="45" t="s">
+      <c r="A111" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="B111" s="34">
+      <c r="B111" s="31">
         <v>109</v>
       </c>
-      <c r="C111" s="45" t="s">
+      <c r="C111" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="D111" s="34">
+      <c r="D111" s="31">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="46" t="s">
+      <c r="A112" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="B112" s="35">
+      <c r="B112" s="32">
         <v>110</v>
       </c>
-      <c r="C112" s="46" t="s">
+      <c r="C112" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D112" s="35">
+      <c r="D112" s="32">
         <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="45" t="s">
+      <c r="A113" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B113" s="34">
+      <c r="B113" s="31">
         <v>111</v>
       </c>
-      <c r="C113" s="45" t="s">
+      <c r="C113" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="D113" s="34">
+      <c r="D113" s="31">
         <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="46" t="s">
+      <c r="A114" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B114" s="35">
+      <c r="B114" s="32">
         <v>112</v>
       </c>
-      <c r="C114" s="46" t="s">
+      <c r="C114" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="D114" s="35">
+      <c r="D114" s="32">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="45" t="s">
+      <c r="A115" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B115" s="34">
+      <c r="B115" s="31">
         <v>113</v>
       </c>
-      <c r="C115" s="45" t="s">
+      <c r="C115" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="D115" s="34">
+      <c r="D115" s="31">
         <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="46" t="s">
+      <c r="A116" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B116" s="35">
+      <c r="B116" s="32">
         <v>114</v>
       </c>
-      <c r="C116" s="46" t="s">
+      <c r="C116" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="D116" s="35">
+      <c r="D116" s="32">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="45" t="s">
+      <c r="A117" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B117" s="34">
+      <c r="B117" s="31">
         <v>115</v>
       </c>
-      <c r="C117" s="45" t="s">
+      <c r="C117" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="D117" s="34">
+      <c r="D117" s="31">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="46" t="s">
+      <c r="A118" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="35">
+      <c r="B118" s="32">
         <v>116</v>
       </c>
-      <c r="C118" s="46" t="s">
+      <c r="C118" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D118" s="35">
+      <c r="D118" s="32">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="45" t="s">
+      <c r="A119" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B119" s="34">
+      <c r="B119" s="31">
         <v>117</v>
       </c>
-      <c r="C119" s="45" t="s">
+      <c r="C119" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="D119" s="34">
+      <c r="D119" s="31">
         <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="46" t="s">
+      <c r="A120" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="B120" s="35">
+      <c r="B120" s="32">
         <v>118</v>
       </c>
-      <c r="C120" s="46" t="s">
+      <c r="C120" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="D120" s="35">
+      <c r="D120" s="32">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="45" t="s">
+      <c r="A121" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B121" s="34">
+      <c r="B121" s="31">
         <v>119</v>
       </c>
-      <c r="C121" s="45" t="s">
+      <c r="C121" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="D121" s="34">
+      <c r="D121" s="31">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="46" t="s">
+      <c r="A122" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="B122" s="35">
+      <c r="B122" s="32">
         <v>120</v>
       </c>
-      <c r="C122" s="46" t="s">
+      <c r="C122" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="D122" s="35">
+      <c r="D122" s="32">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="45" t="s">
+      <c r="A123" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="B123" s="34">
+      <c r="B123" s="31">
         <v>121</v>
       </c>
-      <c r="C123" s="45" t="s">
+      <c r="C123" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="D123" s="34">
+      <c r="D123" s="31">
         <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="46" t="s">
+      <c r="A124" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="B124" s="35">
+      <c r="B124" s="32">
         <v>122</v>
       </c>
-      <c r="C124" s="46" t="s">
+      <c r="C124" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="D124" s="35">
+      <c r="D124" s="32">
         <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="45" t="s">
+      <c r="A125" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="B125" s="34">
+      <c r="B125" s="31">
         <v>123</v>
       </c>
-      <c r="C125" s="45" t="s">
+      <c r="C125" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="D125" s="34">
+      <c r="D125" s="31">
         <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="46" t="s">
+      <c r="A126" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="B126" s="35">
+      <c r="B126" s="32">
         <v>124</v>
       </c>
-      <c r="C126" s="46" t="s">
+      <c r="C126" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="D126" s="35">
+      <c r="D126" s="32">
         <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="45" t="s">
+      <c r="A127" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="B127" s="34">
+      <c r="B127" s="31">
         <v>125</v>
       </c>
-      <c r="C127" s="45" t="s">
+      <c r="C127" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="D127" s="34">
+      <c r="D127" s="31">
         <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="46" t="s">
+      <c r="A128" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="B128" s="35">
+      <c r="B128" s="32">
         <v>126</v>
       </c>
-      <c r="C128" s="46" t="s">
+      <c r="C128" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="D128" s="35">
+      <c r="D128" s="32">
         <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="45" t="s">
+      <c r="A129" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="B129" s="34">
+      <c r="B129" s="31">
         <v>127</v>
       </c>
-      <c r="C129" s="45" t="s">
+      <c r="C129" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="D129" s="34">
+      <c r="D129" s="31">
         <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="46" t="s">
+      <c r="A130" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="B130" s="35">
+      <c r="B130" s="32">
         <v>128</v>
       </c>
-      <c r="C130" s="46" t="s">
+      <c r="C130" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="D130" s="35">
+      <c r="D130" s="32">
         <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="45" t="s">
+      <c r="A131" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="B131" s="34">
+      <c r="B131" s="31">
         <v>129</v>
       </c>
-      <c r="C131" s="45" t="s">
+      <c r="C131" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="D131" s="34">
+      <c r="D131" s="31">
         <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="46" t="s">
+      <c r="A132" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="B132" s="35">
+      <c r="B132" s="32">
         <v>130</v>
       </c>
-      <c r="C132" s="46" t="s">
+      <c r="C132" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="D132" s="35">
+      <c r="D132" s="32">
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="45" t="s">
+      <c r="A133" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="B133" s="34">
+      <c r="B133" s="31">
         <v>131</v>
       </c>
-      <c r="C133" s="45" t="s">
+      <c r="C133" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="D133" s="34">
+      <c r="D133" s="31">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="46" t="s">
+      <c r="A134" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="B134" s="35">
+      <c r="B134" s="32">
         <v>132</v>
       </c>
-      <c r="C134" s="46" t="s">
+      <c r="C134" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D134" s="35">
+      <c r="D134" s="32">
         <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="45" t="s">
+      <c r="A135" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="34">
+      <c r="B135" s="31">
         <v>133</v>
       </c>
-      <c r="C135" s="45" t="s">
+      <c r="C135" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="D135" s="34">
+      <c r="D135" s="31">
         <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="46" t="s">
+      <c r="A136" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="B136" s="35">
+      <c r="B136" s="32">
         <v>134</v>
       </c>
-      <c r="C136" s="46" t="s">
+      <c r="C136" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="D136" s="35">
+      <c r="D136" s="32">
         <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="45" t="s">
+      <c r="A137" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="B137" s="34">
+      <c r="B137" s="31">
         <v>135</v>
       </c>
-      <c r="C137" s="45" t="s">
+      <c r="C137" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="D137" s="34">
+      <c r="D137" s="31">
         <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="46" t="s">
+      <c r="A138" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="B138" s="35">
+      <c r="B138" s="32">
         <v>136</v>
       </c>
-      <c r="C138" s="46" t="s">
+      <c r="C138" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="D138" s="35">
+      <c r="D138" s="32">
         <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="45" t="s">
+      <c r="A139" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="B139" s="34">
+      <c r="B139" s="31">
         <v>137</v>
       </c>
-      <c r="C139" s="45" t="s">
+      <c r="C139" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="D139" s="34">
+      <c r="D139" s="31">
         <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="46" t="s">
+      <c r="A140" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="B140" s="35">
+      <c r="B140" s="32">
         <v>138</v>
       </c>
-      <c r="C140" s="46" t="s">
+      <c r="C140" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="D140" s="35">
+      <c r="D140" s="32">
         <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="45" t="s">
+      <c r="A141" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="B141" s="34">
+      <c r="B141" s="31">
         <v>139</v>
       </c>
-      <c r="C141" s="45" t="s">
+      <c r="C141" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="D141" s="34">
+      <c r="D141" s="31">
         <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="46" t="s">
+      <c r="A142" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="B142" s="35">
+      <c r="B142" s="32">
         <v>140</v>
       </c>
-      <c r="C142" s="46" t="s">
+      <c r="C142" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D142" s="35">
+      <c r="D142" s="32">
         <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="45" t="s">
+      <c r="A143" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="B143" s="34">
+      <c r="B143" s="31">
         <v>141</v>
       </c>
-      <c r="C143" s="45" t="s">
+      <c r="C143" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="D143" s="34">
+      <c r="D143" s="31">
         <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="46" t="s">
+      <c r="A144" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="B144" s="35">
+      <c r="B144" s="32">
         <v>142</v>
       </c>
-      <c r="C144" s="46" t="s">
+      <c r="C144" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="D144" s="35">
+      <c r="D144" s="32">
         <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="45" t="s">
+      <c r="A145" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="B145" s="34">
+      <c r="B145" s="31">
         <v>143</v>
       </c>
-      <c r="C145" s="45" t="s">
+      <c r="C145" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D145" s="34">
+      <c r="D145" s="31">
         <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="46" t="s">
+      <c r="A146" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="B146" s="35">
+      <c r="B146" s="32">
         <v>144</v>
       </c>
-      <c r="C146" s="46" t="s">
+      <c r="C146" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="D146" s="35">
+      <c r="D146" s="32">
         <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="45" t="s">
+      <c r="A147" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="B147" s="34">
+      <c r="B147" s="31">
         <v>145</v>
       </c>
-      <c r="C147" s="45" t="s">
+      <c r="C147" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="D147" s="34">
+      <c r="D147" s="31">
         <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="46" t="s">
+      <c r="A148" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="B148" s="35">
+      <c r="B148" s="32">
         <v>146</v>
       </c>
-      <c r="C148" s="46" t="s">
+      <c r="C148" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="D148" s="35">
+      <c r="D148" s="32">
         <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="45" t="s">
+      <c r="A149" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="B149" s="34">
+      <c r="B149" s="31">
         <v>147</v>
       </c>
-      <c r="C149" s="45" t="s">
+      <c r="C149" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="D149" s="34">
+      <c r="D149" s="31">
         <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="46" t="s">
+      <c r="A150" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="B150" s="35">
+      <c r="B150" s="32">
         <v>148</v>
       </c>
-      <c r="C150" s="46" t="s">
+      <c r="C150" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="D150" s="35">
+      <c r="D150" s="32">
         <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="45" t="s">
+      <c r="A151" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B151" s="34">
+      <c r="B151" s="31">
         <v>149</v>
       </c>
-      <c r="C151" s="45" t="s">
+      <c r="C151" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="D151" s="34">
+      <c r="D151" s="31">
         <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="46" t="s">
+      <c r="A152" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="B152" s="35">
+      <c r="B152" s="32">
         <v>150</v>
       </c>
-      <c r="C152" s="46" t="s">
+      <c r="C152" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="D152" s="35">
+      <c r="D152" s="32">
         <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="45" t="s">
+      <c r="A153" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="B153" s="34">
+      <c r="B153" s="31">
         <v>151</v>
       </c>
-      <c r="C153" s="45" t="s">
+      <c r="C153" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="D153" s="34">
+      <c r="D153" s="31">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="46" t="s">
+      <c r="A154" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="B154" s="35">
+      <c r="B154" s="32">
         <v>152</v>
       </c>
-      <c r="C154" s="46" t="s">
+      <c r="C154" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="D154" s="35">
+      <c r="D154" s="32">
         <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="45" t="s">
+      <c r="A155" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="B155" s="34">
+      <c r="B155" s="31">
         <v>153</v>
       </c>
-      <c r="C155" s="45" t="s">
+      <c r="C155" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="D155" s="34">
+      <c r="D155" s="31">
         <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="46" t="s">
+      <c r="A156" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="B156" s="35">
+      <c r="B156" s="32">
         <v>154</v>
       </c>
-      <c r="C156" s="46" t="s">
+      <c r="C156" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="D156" s="35">
+      <c r="D156" s="32">
         <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="45" t="s">
+      <c r="A157" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="B157" s="34">
+      <c r="B157" s="31">
         <v>155</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="C157" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="D157" s="34">
+      <c r="D157" s="31">
         <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="46" t="s">
+      <c r="A158" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="B158" s="35">
+      <c r="B158" s="32">
         <v>156</v>
       </c>
-      <c r="C158" s="46" t="s">
+      <c r="C158" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="D158" s="35">
+      <c r="D158" s="32">
         <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="45" t="s">
+      <c r="A159" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="B159" s="34">
+      <c r="B159" s="31">
         <v>157</v>
       </c>
-      <c r="C159" s="45" t="s">
+      <c r="C159" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D159" s="34">
+      <c r="D159" s="31">
         <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="46" t="s">
+      <c r="A160" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="B160" s="35">
+      <c r="B160" s="32">
         <v>158</v>
       </c>
-      <c r="C160" s="46" t="s">
+      <c r="C160" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="D160" s="35">
+      <c r="D160" s="32">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="45" t="s">
+      <c r="A161" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="B161" s="34">
+      <c r="B161" s="31">
         <v>159</v>
       </c>
-      <c r="C161" s="45" t="s">
+      <c r="C161" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="D161" s="34">
+      <c r="D161" s="31">
         <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="46" t="s">
+      <c r="A162" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="B162" s="35">
+      <c r="B162" s="32">
         <v>160</v>
       </c>
-      <c r="C162" s="46" t="s">
+      <c r="C162" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="D162" s="35">
+      <c r="D162" s="32">
         <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="45" t="s">
+      <c r="A163" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="B163" s="34">
+      <c r="B163" s="31">
         <v>161</v>
       </c>
-      <c r="C163" s="45" t="s">
+      <c r="C163" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="D163" s="34">
+      <c r="D163" s="31">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="46" t="s">
+      <c r="A164" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="B164" s="35">
+      <c r="B164" s="32">
         <v>162</v>
       </c>
-      <c r="C164" s="46" t="s">
+      <c r="C164" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="D164" s="35">
+      <c r="D164" s="32">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="45" t="s">
+      <c r="A165" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B165" s="34">
+      <c r="B165" s="31">
         <v>163</v>
       </c>
-      <c r="C165" s="45" t="s">
+      <c r="C165" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="D165" s="34">
+      <c r="D165" s="31">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="46" t="s">
+      <c r="A166" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="B166" s="35">
+      <c r="B166" s="32">
         <v>164</v>
       </c>
-      <c r="C166" s="46" t="s">
+      <c r="C166" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="D166" s="35">
+      <c r="D166" s="32">
         <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="45" t="s">
+      <c r="A167" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="B167" s="34">
+      <c r="B167" s="31">
         <v>165</v>
       </c>
-      <c r="C167" s="45" t="s">
+      <c r="C167" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D167" s="34">
+      <c r="D167" s="31">
         <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="46" t="s">
+      <c r="A168" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="B168" s="35">
+      <c r="B168" s="32">
         <v>166</v>
       </c>
-      <c r="C168" s="46" t="s">
+      <c r="C168" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="D168" s="35">
+      <c r="D168" s="32">
         <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="45" t="s">
+      <c r="A169" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B169" s="34">
+      <c r="B169" s="31">
         <v>167</v>
       </c>
-      <c r="C169" s="45" t="s">
+      <c r="C169" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="D169" s="34">
+      <c r="D169" s="31">
         <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="46" t="s">
+      <c r="A170" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="B170" s="35">
+      <c r="B170" s="32">
         <v>168</v>
       </c>
-      <c r="C170" s="46" t="s">
+      <c r="C170" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D170" s="35">
+      <c r="D170" s="32">
         <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="45" t="s">
+      <c r="A171" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="B171" s="34">
+      <c r="B171" s="31">
         <v>169</v>
       </c>
-      <c r="C171" s="45" t="s">
+      <c r="C171" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="D171" s="34">
+      <c r="D171" s="31">
         <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="46" t="s">
+      <c r="A172" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="B172" s="35">
+      <c r="B172" s="32">
         <v>170</v>
       </c>
-      <c r="C172" s="46" t="s">
+      <c r="C172" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="D172" s="35">
+      <c r="D172" s="32">
         <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="45" t="s">
+      <c r="A173" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="B173" s="34">
+      <c r="B173" s="31">
         <v>171</v>
       </c>
-      <c r="C173" s="45" t="s">
+      <c r="C173" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="D173" s="34">
+      <c r="D173" s="31">
         <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="46" t="s">
+      <c r="A174" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="B174" s="35">
+      <c r="B174" s="32">
         <v>172</v>
       </c>
-      <c r="C174" s="46" t="s">
+      <c r="C174" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="D174" s="35">
+      <c r="D174" s="32">
         <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="45" t="s">
+      <c r="A175" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="B175" s="34">
+      <c r="B175" s="31">
         <v>173</v>
       </c>
-      <c r="C175" s="45" t="s">
+      <c r="C175" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="34">
+      <c r="D175" s="31">
         <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="46" t="s">
+      <c r="A176" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B176" s="35">
+      <c r="B176" s="32">
         <v>174</v>
       </c>
-      <c r="C176" s="46" t="s">
+      <c r="C176" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="D176" s="35">
+      <c r="D176" s="32">
         <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="45" t="s">
+      <c r="A177" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="B177" s="34">
+      <c r="B177" s="31">
         <v>175</v>
       </c>
-      <c r="C177" s="45" t="s">
+      <c r="C177" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="D177" s="34">
+      <c r="D177" s="31">
         <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="46" t="s">
+      <c r="A178" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="B178" s="35">
+      <c r="B178" s="32">
         <v>176</v>
       </c>
-      <c r="C178" s="46" t="s">
+      <c r="C178" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D178" s="35">
+      <c r="D178" s="32">
         <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="45" t="s">
+      <c r="A179" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="B179" s="34">
+      <c r="B179" s="31">
         <v>177</v>
       </c>
-      <c r="C179" s="45" t="s">
+      <c r="C179" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="D179" s="34">
+      <c r="D179" s="31">
         <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="46" t="s">
+      <c r="A180" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="B180" s="35">
+      <c r="B180" s="32">
         <v>178</v>
       </c>
-      <c r="C180" s="46" t="s">
+      <c r="C180" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="D180" s="35">
+      <c r="D180" s="32">
         <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="45" t="s">
+      <c r="A181" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="B181" s="34">
+      <c r="B181" s="31">
         <v>179</v>
       </c>
-      <c r="C181" s="45" t="s">
+      <c r="C181" s="42" t="s">
         <v>268</v>
       </c>
-      <c r="D181" s="34">
+      <c r="D181" s="31">
         <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="46" t="s">
+      <c r="A182" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="B182" s="35">
+      <c r="B182" s="32">
         <v>180</v>
       </c>
-      <c r="C182" s="46" t="s">
+      <c r="C182" s="43" t="s">
         <v>269</v>
       </c>
-      <c r="D182" s="35">
+      <c r="D182" s="32">
         <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="45" t="s">
+      <c r="A183" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="B183" s="34">
+      <c r="B183" s="31">
         <v>181</v>
       </c>
-      <c r="C183" s="45" t="s">
+      <c r="C183" s="42" t="s">
         <v>270</v>
       </c>
-      <c r="D183" s="34">
+      <c r="D183" s="31">
         <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="46" t="s">
+      <c r="A184" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="B184" s="35">
+      <c r="B184" s="32">
         <v>182</v>
       </c>
-      <c r="C184" s="46" t="s">
+      <c r="C184" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="D184" s="35">
+      <c r="D184" s="32">
         <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="45" t="s">
+      <c r="A185" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="B185" s="34">
+      <c r="B185" s="31">
         <v>183</v>
       </c>
-      <c r="C185" s="45" t="s">
+      <c r="C185" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="D185" s="34">
+      <c r="D185" s="31">
         <v>183</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="46" t="s">
+      <c r="A186" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="B186" s="35">
+      <c r="B186" s="32">
         <v>184</v>
       </c>
-      <c r="C186" s="47" t="s">
+      <c r="C186" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="D186" s="36">
+      <c r="D186" s="33">
         <v>184</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="45" t="s">
+      <c r="A187" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="B187" s="34">
+      <c r="B187" s="31">
         <v>185</v>
       </c>
-      <c r="C187" s="45" t="s">
+      <c r="C187" s="42" t="s">
         <v>272</v>
       </c>
-      <c r="D187" s="34">
+      <c r="D187" s="31">
         <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="46" t="s">
+      <c r="A188" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="B188" s="35">
+      <c r="B188" s="32">
         <v>186</v>
       </c>
-      <c r="C188" s="46" t="s">
+      <c r="C188" s="43" t="s">
         <v>273</v>
       </c>
-      <c r="D188" s="35">
+      <c r="D188" s="32">
         <v>186</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="45" t="s">
+      <c r="A189" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="B189" s="34">
+      <c r="B189" s="31">
         <v>187</v>
       </c>
-      <c r="C189" s="45" t="s">
+      <c r="C189" s="42" t="s">
         <v>274</v>
       </c>
-      <c r="D189" s="34">
+      <c r="D189" s="31">
         <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="46" t="s">
+      <c r="A190" s="43" t="s">
         <v>238</v>
       </c>
-      <c r="B190" s="35">
+      <c r="B190" s="32">
         <v>188</v>
       </c>
-      <c r="C190" s="46" t="s">
+      <c r="C190" s="43" t="s">
         <v>275</v>
       </c>
-      <c r="D190" s="35">
+      <c r="D190" s="32">
         <v>188</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="45" t="s">
+      <c r="A191" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="B191" s="34">
+      <c r="B191" s="31">
         <v>189</v>
       </c>
-      <c r="C191" s="45" t="s">
+      <c r="C191" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="D191" s="34">
+      <c r="D191" s="31">
         <v>189</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="46" t="s">
+      <c r="A192" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="B192" s="35">
+      <c r="B192" s="32">
         <v>190</v>
       </c>
-      <c r="C192" s="46" t="s">
+      <c r="C192" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="D192" s="35">
+      <c r="D192" s="32">
         <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="45" t="s">
+      <c r="A193" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="B193" s="34">
+      <c r="B193" s="31">
         <v>191</v>
       </c>
-      <c r="C193" s="45" t="s">
+      <c r="C193" s="42" t="s">
         <v>276</v>
       </c>
-      <c r="D193" s="34">
+      <c r="D193" s="31">
         <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="46" t="s">
+      <c r="A194" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="B194" s="35">
+      <c r="B194" s="32">
         <v>192</v>
       </c>
-      <c r="C194" s="46" t="s">
+      <c r="C194" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="D194" s="35">
+      <c r="D194" s="32">
         <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="45" t="s">
+      <c r="A195" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="B195" s="34">
+      <c r="B195" s="31">
         <v>193</v>
       </c>
-      <c r="C195" s="45" t="s">
+      <c r="C195" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="D195" s="34">
+      <c r="D195" s="31">
         <v>193</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="46" t="s">
+      <c r="A196" s="43" t="s">
         <v>244</v>
       </c>
-      <c r="B196" s="35">
+      <c r="B196" s="32">
         <v>194</v>
       </c>
-      <c r="C196" s="46" t="s">
+      <c r="C196" s="43" t="s">
         <v>277</v>
       </c>
-      <c r="D196" s="35">
+      <c r="D196" s="32">
         <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="45" t="s">
+      <c r="A197" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="B197" s="34">
+      <c r="B197" s="31">
         <v>195</v>
       </c>
-      <c r="C197" s="45" t="s">
+      <c r="C197" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="D197" s="34">
+      <c r="D197" s="31">
         <v>195</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="46" t="s">
+      <c r="A198" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B198" s="35">
+      <c r="B198" s="32">
         <v>196</v>
       </c>
-      <c r="C198" s="46" t="s">
+      <c r="C198" s="43" t="s">
         <v>278</v>
       </c>
-      <c r="D198" s="35">
+      <c r="D198" s="32">
         <v>196</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="45" t="s">
+      <c r="A199" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="B199" s="34">
+      <c r="B199" s="31">
         <v>197</v>
       </c>
-      <c r="C199" s="45" t="s">
+      <c r="C199" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="D199" s="34">
+      <c r="D199" s="31">
         <v>197</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="46" t="s">
+      <c r="A200" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="B200" s="35">
+      <c r="B200" s="32">
         <v>198</v>
       </c>
-      <c r="C200" s="46" t="s">
+      <c r="C200" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="D200" s="35">
+      <c r="D200" s="32">
         <v>198</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="45" t="s">
+      <c r="A201" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="B201" s="34">
+      <c r="B201" s="31">
         <v>199</v>
       </c>
-      <c r="C201" s="45" t="s">
+      <c r="C201" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="D201" s="34">
+      <c r="D201" s="31">
         <v>199</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="47" t="s">
+      <c r="A202" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="B202" s="36">
+      <c r="B202" s="33">
         <v>200</v>
       </c>
-      <c r="C202" s="46" t="s">
+      <c r="C202" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="D202" s="35">
+      <c r="D202" s="32">
         <v>200</v>
       </c>
     </row>

</xml_diff>